<commit_message>
add RKI data downloaded 2020-11-05--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Testzahlen-gesamt.xlsx
+++ b/rki-data/RKI-Testzahlen-gesamt.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="810" windowWidth="19440" windowHeight="11040" tabRatio="301" activeTab="2"/>
+    <workbookView xWindow="690" yWindow="810" windowWidth="19440" windowHeight="11040" tabRatio="301"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterungen" sheetId="5" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Testkapazitäten" sheetId="2" r:id="rId3"/>
     <sheet name="Probenrückstau" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Kalenderwoche 2020</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>KW44</t>
+  </si>
+  <si>
+    <t>KW45</t>
   </si>
 </sst>
 </file>
@@ -488,6 +491,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -531,9 +535,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Probenrückstau!$A$2:$B$30</c:f>
+              <c:f>Probenrückstau!$A$2:$B$31</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>15</c:v>
@@ -621,6 +625,9 @@
                   </c:pt>
                   <c:pt idx="28">
                     <c:v>43</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>44</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -710,6 +717,9 @@
                   </c:pt>
                   <c:pt idx="28">
                     <c:v>57</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>69</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -717,10 +727,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Probenrückstau!$C$2:$C$30</c:f>
+              <c:f>Probenrückstau!$C$2:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>3423</c:v>
                 </c:pt>
@@ -808,6 +818,9 @@
                 <c:pt idx="28">
                   <c:v>68574</c:v>
                 </c:pt>
+                <c:pt idx="29">
+                  <c:v>98931</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -826,11 +839,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="91584000"/>
-        <c:axId val="91585920"/>
+        <c:axId val="114662400"/>
+        <c:axId val="114987008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91584000"/>
+        <c:axId val="114662400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -879,7 +892,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91585920"/>
+        <c:crossAx val="114987008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -887,7 +900,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91585920"/>
+        <c:axId val="114987008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,13 +922,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91584000"/>
+        <c:crossAx val="114662400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -952,7 +966,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1264,7 +1278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:A5"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1298,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,7 +1370,7 @@
         <v>7582</v>
       </c>
       <c r="E5" s="24">
-        <f t="shared" ref="E5:E37" si="0">(D5/C5)*100</f>
+        <f t="shared" ref="E5:E38" si="0">(D5/C5)*100</f>
         <v>5.9486728857575502</v>
       </c>
       <c r="F5" s="13">
@@ -1512,17 +1526,17 @@
         <v>20</v>
       </c>
       <c r="C14" s="20">
-        <v>432666</v>
+        <v>432076</v>
       </c>
       <c r="D14" s="20">
-        <v>7233</v>
+        <v>7080</v>
       </c>
       <c r="E14" s="24">
-        <f>(D14/C14)*100</f>
-        <v>1.6717283077477778</v>
+        <f t="shared" si="0"/>
+        <v>1.6386006165581981</v>
       </c>
       <c r="F14" s="19">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1530,17 +1544,17 @@
         <v>21</v>
       </c>
       <c r="C15" s="20">
-        <v>353467</v>
+        <v>354260</v>
       </c>
       <c r="D15" s="20">
-        <v>5218</v>
+        <v>5228</v>
       </c>
       <c r="E15" s="24">
         <f t="shared" si="0"/>
-        <v>1.4762339907261497</v>
+        <v>1.4757522723423475</v>
       </c>
       <c r="F15" s="19">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1548,17 +1562,17 @@
         <v>22</v>
       </c>
       <c r="C16" s="20">
-        <v>405269</v>
+        <v>401589</v>
       </c>
       <c r="D16" s="20">
-        <v>4310</v>
+        <v>4267</v>
       </c>
       <c r="E16" s="24">
         <f t="shared" si="0"/>
-        <v>1.0634911626598629</v>
+        <v>1.0625291031377853</v>
       </c>
       <c r="F16" s="19">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1566,17 +1580,17 @@
         <v>23</v>
       </c>
       <c r="C17" s="20">
-        <v>340986</v>
+        <v>337217</v>
       </c>
       <c r="D17" s="20">
-        <v>3208</v>
+        <v>3085</v>
       </c>
       <c r="E17" s="24">
         <f t="shared" si="0"/>
-        <v>0.94080108860774347</v>
+        <v>0.9148411853494931</v>
       </c>
       <c r="F17" s="19">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -1602,17 +1616,17 @@
         <v>25</v>
       </c>
       <c r="C19" s="20">
-        <v>388187</v>
+        <v>386316</v>
       </c>
       <c r="D19" s="20">
-        <v>5316</v>
+        <v>5276</v>
       </c>
       <c r="E19" s="24">
         <f t="shared" si="0"/>
-        <v>1.3694430776919371</v>
+        <v>1.3657213265823833</v>
       </c>
       <c r="F19" s="19">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1620,17 +1634,17 @@
         <v>26</v>
       </c>
       <c r="C20" s="20">
-        <v>467413</v>
+        <v>464626</v>
       </c>
       <c r="D20" s="20">
-        <v>3689</v>
+        <v>3682</v>
       </c>
       <c r="E20" s="24">
         <f t="shared" si="0"/>
-        <v>0.78923778328801297</v>
+        <v>0.79246533771248284</v>
       </c>
       <c r="F20" s="19">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -1638,17 +1652,17 @@
         <v>27</v>
       </c>
       <c r="C21" s="20">
-        <v>507663</v>
+        <v>506459</v>
       </c>
       <c r="D21" s="20">
-        <v>3104</v>
+        <v>3092</v>
       </c>
       <c r="E21" s="24">
         <f t="shared" si="0"/>
-        <v>0.61142923553617268</v>
+        <v>0.61051338805312971</v>
       </c>
       <c r="F21" s="19">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1692,17 +1706,17 @@
         <v>30</v>
       </c>
       <c r="C24" s="20">
-        <v>574883</v>
+        <v>553429</v>
       </c>
       <c r="D24" s="20">
-        <v>4539</v>
+        <v>4458</v>
       </c>
       <c r="E24" s="24">
         <f t="shared" si="0"/>
-        <v>0.78955196100771818</v>
+        <v>0.80552338240316279</v>
       </c>
       <c r="F24" s="19">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -1728,17 +1742,17 @@
         <v>32</v>
       </c>
       <c r="C26" s="20">
-        <v>736171</v>
+        <v>716768</v>
       </c>
       <c r="D26" s="20">
-        <v>7335</v>
+        <v>7263</v>
       </c>
       <c r="E26" s="24">
         <f t="shared" si="0"/>
-        <v>0.99637176688568285</v>
+        <v>1.0132985847582481</v>
       </c>
       <c r="F26" s="19">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -1746,17 +1760,17 @@
         <v>33</v>
       </c>
       <c r="C27" s="20">
-        <v>857761</v>
+        <v>835384</v>
       </c>
       <c r="D27" s="20">
-        <v>8351</v>
+        <v>8121</v>
       </c>
       <c r="E27" s="24">
         <f t="shared" si="0"/>
-        <v>0.9735812190108899</v>
+        <v>0.97212778793943855</v>
       </c>
       <c r="F27" s="19">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -1764,17 +1778,17 @@
         <v>34</v>
       </c>
       <c r="C28" s="20">
-        <v>1092013</v>
+        <v>1084446</v>
       </c>
       <c r="D28" s="20">
-        <v>9206</v>
+        <v>9143</v>
       </c>
       <c r="E28" s="24">
         <f t="shared" si="0"/>
-        <v>0.84303025696580536</v>
+        <v>0.84310329882723523</v>
       </c>
       <c r="F28" s="19">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -1782,17 +1796,17 @@
         <v>35</v>
       </c>
       <c r="C29" s="20">
-        <v>1121214</v>
+        <v>1120883</v>
       </c>
       <c r="D29" s="20">
-        <v>8324</v>
+        <v>8323</v>
       </c>
       <c r="E29" s="24">
         <f t="shared" si="0"/>
-        <v>0.74240956677315839</v>
+        <v>0.74253958709338974</v>
       </c>
       <c r="F29" s="19">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -1800,17 +1814,17 @@
         <v>36</v>
       </c>
       <c r="C30" s="20">
-        <v>1099608</v>
+        <v>1072316</v>
       </c>
       <c r="D30" s="20">
-        <v>8175</v>
+        <v>8294</v>
       </c>
       <c r="E30" s="24">
         <f t="shared" si="0"/>
-        <v>0.7434467555710762</v>
+        <v>0.7734660305357749</v>
       </c>
       <c r="F30" s="19">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -1818,17 +1832,17 @@
         <v>37</v>
       </c>
       <c r="C31" s="20">
-        <v>1165275</v>
+        <v>1164932</v>
       </c>
       <c r="D31" s="20">
-        <v>10047</v>
+        <v>10046</v>
       </c>
       <c r="E31" s="24">
         <f t="shared" si="0"/>
-        <v>0.8621999098925146</v>
+        <v>0.86236793220548502</v>
       </c>
       <c r="F31" s="19">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -1836,17 +1850,17 @@
         <v>38</v>
       </c>
       <c r="C32" s="20">
-        <v>1146193</v>
+        <v>1146565</v>
       </c>
       <c r="D32" s="20">
-        <v>13253</v>
+        <v>13261</v>
       </c>
       <c r="E32" s="24">
         <f t="shared" si="0"/>
-        <v>1.1562625142537077</v>
+        <v>1.156585104202553</v>
       </c>
       <c r="F32" s="19">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -1854,17 +1868,17 @@
         <v>39</v>
       </c>
       <c r="C33" s="20">
-        <v>1168016</v>
+        <v>1155995</v>
       </c>
       <c r="D33" s="20">
-        <v>14295</v>
+        <v>14094</v>
       </c>
       <c r="E33" s="24">
         <f t="shared" si="0"/>
-        <v>1.2238702209558774</v>
+        <v>1.2192094256463049</v>
       </c>
       <c r="F33" s="19">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -1872,17 +1886,17 @@
         <v>40</v>
       </c>
       <c r="C34" s="20">
-        <v>1101080</v>
+        <v>1101413</v>
       </c>
       <c r="D34" s="20">
-        <v>18279</v>
+        <v>18290</v>
       </c>
       <c r="E34" s="24">
         <f t="shared" si="0"/>
-        <v>1.6600973589566608</v>
+        <v>1.6605941640420077</v>
       </c>
       <c r="F34" s="19">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -1890,17 +1904,17 @@
         <v>41</v>
       </c>
       <c r="C35" s="20">
-        <v>1213658</v>
+        <v>1188338</v>
       </c>
       <c r="D35" s="20">
-        <v>30519</v>
+        <v>29567</v>
       </c>
       <c r="E35" s="24">
         <f t="shared" si="0"/>
-        <v>2.5146293272075</v>
+        <v>2.4880968209381504</v>
       </c>
       <c r="F35" s="19">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -1908,17 +1922,17 @@
         <v>42</v>
       </c>
       <c r="C36" s="20">
-        <v>1212363</v>
+        <v>1261398</v>
       </c>
       <c r="D36" s="20">
-        <v>43927</v>
+        <v>44733</v>
       </c>
       <c r="E36" s="24">
         <f t="shared" si="0"/>
-        <v>3.6232547512584929</v>
+        <v>3.5463033871942087</v>
       </c>
       <c r="F36" s="19">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -1926,33 +1940,51 @@
         <v>43</v>
       </c>
       <c r="C37" s="20">
-        <v>1358706</v>
+        <v>1401443</v>
       </c>
       <c r="D37" s="20">
-        <v>76373</v>
+        <v>77168</v>
       </c>
       <c r="E37" s="24">
         <f t="shared" si="0"/>
-        <v>5.6210099903879129</v>
+        <v>5.5063245526218338</v>
       </c>
       <c r="F37" s="19">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="19">
+        <v>44</v>
+      </c>
+      <c r="C38" s="20">
+        <v>1567083</v>
+      </c>
+      <c r="D38" s="20">
+        <v>113822</v>
+      </c>
+      <c r="E38" s="24">
+        <f t="shared" si="0"/>
+        <v>7.2633038581874727</v>
+      </c>
+      <c r="F38" s="19">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="22">
-        <f>SUM(C4:C37)</f>
-        <v>21882967</v>
-      </c>
-      <c r="D38" s="22">
-        <f>SUM(D4:D37)</f>
-        <v>497656</v>
-      </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
+      <c r="C39" s="22">
+        <f>SUM(C4:C38)</f>
+        <v>23393311</v>
+      </c>
+      <c r="D39" s="22">
+        <f>SUM(D4:D38)</f>
+        <v>611248</v>
+      </c>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
@@ -1963,7 +1995,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1972,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E36"/>
+  <dimension ref="A2:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,6 +2614,23 @@
         <v>1612826</v>
       </c>
     </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="31">
+        <v>176</v>
+      </c>
+      <c r="C37" s="29">
+        <v>289310</v>
+      </c>
+      <c r="D37" s="29">
+        <v>1900642</v>
+      </c>
+      <c r="E37" s="35">
+        <v>1596042</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2589,10 +2638,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2956,6 +3005,17 @@
         <v>68574</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="34">
+        <v>69</v>
+      </c>
+      <c r="B31" s="34">
+        <v>44</v>
+      </c>
+      <c r="C31" s="35">
+        <v>98931</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add RKI data downloaded 2020-12-24--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Testzahlen-gesamt.xlsx
+++ b/rki-data/RKI-Testzahlen-gesamt.xlsx
@@ -1,11 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20368"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF2375D0-B47F-4401-811D-D22328E44FAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="3810" windowWidth="19440" windowHeight="11040" tabRatio="301"/>
+    <workbookView xWindow="690" yWindow="3810" windowWidth="19440" windowHeight="11040" tabRatio="301" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterungen" sheetId="5" r:id="rId1"/>
@@ -13,12 +14,12 @@
     <sheet name="Testkapazitäten" sheetId="2" r:id="rId3"/>
     <sheet name="Probenrückstau" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Kalenderwoche 2020</t>
   </si>
@@ -213,12 +214,18 @@
   </si>
   <si>
     <t>KW51</t>
+  </si>
+  <si>
+    <t>51*</t>
+  </si>
+  <si>
+    <t>KW52</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;\ _€_-;_-@_-"/>
@@ -477,29 +484,29 @@
     </xf>
   </cellXfs>
   <cellStyles count="23">
-    <cellStyle name="Comma" xfId="5"/>
-    <cellStyle name="Comma [0]" xfId="6"/>
-    <cellStyle name="Currency" xfId="3"/>
-    <cellStyle name="Currency [0]" xfId="4"/>
-    <cellStyle name="Hyperlink 2" xfId="11"/>
-    <cellStyle name="Normal" xfId="7"/>
-    <cellStyle name="Percent" xfId="2"/>
+    <cellStyle name="Comma" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma [0]" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Currency" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Currency [0]" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Percent" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 10" xfId="19"/>
-    <cellStyle name="Standard 11" xfId="20"/>
-    <cellStyle name="Standard 12" xfId="21"/>
-    <cellStyle name="Standard 2" xfId="8"/>
-    <cellStyle name="Standard 3" xfId="9"/>
-    <cellStyle name="Standard 4" xfId="10"/>
-    <cellStyle name="Standard 5" xfId="12"/>
-    <cellStyle name="Standard 5 2" xfId="13"/>
-    <cellStyle name="Standard 5 2 2" xfId="22"/>
-    <cellStyle name="Standard 5 3" xfId="14"/>
-    <cellStyle name="Standard 5_Tabelle1" xfId="15"/>
-    <cellStyle name="Standard 6" xfId="1"/>
-    <cellStyle name="Standard 7" xfId="16"/>
-    <cellStyle name="Standard 8" xfId="17"/>
-    <cellStyle name="Standard 9" xfId="18"/>
+    <cellStyle name="Standard 10" xfId="19" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Standard 11" xfId="20" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Standard 12" xfId="21" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Standard 2" xfId="8" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Standard 3" xfId="9" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Standard 4" xfId="10" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Standard 5" xfId="12" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Standard 5 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Standard 5 2 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Standard 5 3" xfId="14" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Standard 5_Tabelle1" xfId="15" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Standard 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Standard 7" xfId="16" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Standard 8" xfId="17" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Standard 9" xfId="18" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -507,12 +514,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -526,7 +536,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -570,9 +579,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Probenrückstau!$A$2:$B$37</c:f>
+              <c:f>Probenrückstau!$A$2:$B$38</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>15</c:v>
@@ -681,6 +690,9 @@
                   </c:pt>
                   <c:pt idx="35">
                     <c:v>50</c:v>
+                  </c:pt>
+                  <c:pt idx="36">
+                    <c:v>51</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -791,6 +803,9 @@
                   </c:pt>
                   <c:pt idx="35">
                     <c:v>50</c:v>
+                  </c:pt>
+                  <c:pt idx="36">
+                    <c:v>57</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -798,10 +813,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Probenrückstau!$C$2:$C$37</c:f>
+              <c:f>Probenrückstau!$C$2:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>3423</c:v>
                 </c:pt>
@@ -909,11 +924,14 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>19009</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>21364.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-68D1-41B7-9863-0787141F2504}"/>
             </c:ext>
@@ -1011,7 +1029,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="0"/>
@@ -1055,7 +1072,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1079,9 +1096,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1119,9 +1136,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1154,9 +1171,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1189,9 +1223,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1364,29 +1415,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="140.85546875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="140.81640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" s="1" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" s="1" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="126" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>48</v>
       </c>
@@ -1398,22 +1449,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B3:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+    <col min="6" max="6" width="20.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
@@ -1430,7 +1481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
@@ -1448,7 +1499,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="11">
         <v>11</v>
       </c>
@@ -1459,14 +1510,14 @@
         <v>7582</v>
       </c>
       <c r="E5" s="22">
-        <f t="shared" ref="E5:E36" si="0">(D5/C5)*100</f>
+        <f t="shared" ref="E5:E12" si="0">(D5/C5)*100</f>
         <v>5.9486728857575502</v>
       </c>
       <c r="F5" s="11">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>12</v>
       </c>
@@ -1484,7 +1535,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="13">
         <v>13</v>
       </c>
@@ -1502,7 +1553,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="19">
         <v>14</v>
       </c>
@@ -1520,7 +1571,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="19">
         <v>15</v>
       </c>
@@ -1538,7 +1589,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="19">
         <v>16</v>
       </c>
@@ -1556,7 +1607,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="17">
         <v>17</v>
       </c>
@@ -1574,7 +1625,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="17">
         <v>18</v>
       </c>
@@ -1592,7 +1643,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="17">
         <v>19</v>
       </c>
@@ -1610,7 +1661,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="2:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="17">
         <v>20</v>
       </c>
@@ -1621,14 +1672,14 @@
         <v>7080</v>
       </c>
       <c r="E14" s="22">
-        <f t="shared" ref="E14:E44" si="1">(D14/C14)*100</f>
+        <f t="shared" ref="E14:E45" si="1">(D14/C14)*100</f>
         <v>1.6386006165581981</v>
       </c>
       <c r="F14" s="17">
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B15" s="17">
         <v>21</v>
       </c>
@@ -1646,7 +1697,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B16" s="17">
         <v>22</v>
       </c>
@@ -1664,7 +1715,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="17">
         <v>23</v>
       </c>
@@ -1682,7 +1733,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="17">
         <v>24</v>
       </c>
@@ -1700,7 +1751,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="17">
         <v>25</v>
       </c>
@@ -1718,7 +1769,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="17">
         <v>26</v>
       </c>
@@ -1736,7 +1787,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="17">
         <v>27</v>
       </c>
@@ -1754,7 +1805,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="17">
         <v>28</v>
       </c>
@@ -1772,7 +1823,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="17">
         <v>29</v>
       </c>
@@ -1790,7 +1841,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="17">
         <v>30</v>
       </c>
@@ -1808,7 +1859,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="17">
         <v>31</v>
       </c>
@@ -1826,7 +1877,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="17">
         <v>32</v>
       </c>
@@ -1844,7 +1895,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="17">
         <v>33</v>
       </c>
@@ -1862,7 +1913,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="17">
         <v>34</v>
       </c>
@@ -1880,7 +1931,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="17">
         <v>35</v>
       </c>
@@ -1898,7 +1949,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="17">
         <v>36</v>
       </c>
@@ -1916,7 +1967,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" s="17">
         <v>37</v>
       </c>
@@ -1934,7 +1985,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B32" s="17">
         <v>38</v>
       </c>
@@ -1952,7 +2003,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B33" s="17">
         <v>39</v>
       </c>
@@ -1970,7 +2021,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B34" s="17">
         <v>40</v>
       </c>
@@ -1988,7 +2039,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B35" s="17">
         <v>41</v>
       </c>
@@ -2006,7 +2057,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36" s="17">
         <v>42</v>
       </c>
@@ -2024,7 +2075,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B37" s="17">
         <v>43</v>
       </c>
@@ -2042,7 +2093,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B38" s="17">
         <v>44</v>
       </c>
@@ -2060,7 +2111,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B39" s="17">
         <v>45</v>
       </c>
@@ -2078,124 +2129,142 @@
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B40" s="17" t="s">
         <v>54</v>
       </c>
       <c r="C40" s="33">
-        <v>1396088</v>
+        <v>1422301</v>
       </c>
       <c r="D40" s="33">
-        <v>125200</v>
+        <v>126181</v>
       </c>
       <c r="E40" s="22">
         <f t="shared" si="1"/>
-        <v>8.967916062597773</v>
+        <v>8.8716101584685667</v>
       </c>
       <c r="F40" s="32">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B41" s="17" t="s">
         <v>55</v>
       </c>
       <c r="C41" s="33">
-        <v>1363701</v>
+        <v>1394255</v>
       </c>
       <c r="D41" s="33">
-        <v>127330</v>
+        <v>128668</v>
       </c>
       <c r="E41" s="22">
         <f t="shared" si="1"/>
-        <v>9.3370907552315341</v>
+        <v>9.2284409953702884</v>
       </c>
       <c r="F41" s="32">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B42" s="17" t="s">
         <v>57</v>
       </c>
       <c r="C42" s="33">
-        <v>1343157</v>
+        <v>1373055</v>
       </c>
       <c r="D42" s="33">
-        <v>124687</v>
+        <v>125752</v>
       </c>
       <c r="E42" s="22">
         <f t="shared" si="1"/>
-        <v>9.283129224655049</v>
+        <v>9.1585551926179214</v>
       </c>
       <c r="F42" s="32">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B43" s="17" t="s">
         <v>60</v>
       </c>
       <c r="C43" s="33">
-        <v>1308629</v>
+        <v>1340025</v>
       </c>
       <c r="D43" s="33">
-        <v>133681</v>
+        <v>134793</v>
       </c>
       <c r="E43" s="22">
         <f t="shared" si="1"/>
-        <v>10.215347512549393</v>
+        <v>10.058991436726927</v>
       </c>
       <c r="F43" s="32">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B44" s="17" t="s">
         <v>63</v>
       </c>
       <c r="C44" s="33">
-        <v>1465732</v>
+        <v>1503685</v>
       </c>
       <c r="D44" s="33">
-        <v>168483</v>
+        <v>170141</v>
       </c>
       <c r="E44" s="22">
         <f t="shared" si="1"/>
-        <v>11.494802596927677</v>
+        <v>11.314936306473763</v>
       </c>
       <c r="F44" s="32">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B45" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="33">
+        <v>1578209</v>
+      </c>
+      <c r="D45" s="33">
+        <v>184156</v>
+      </c>
+      <c r="E45" s="22">
+        <f t="shared" si="1"/>
+        <v>11.668669992377435</v>
+      </c>
+      <c r="F45" s="32">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="20">
-        <f>SUM(C4:C44)</f>
-        <v>31974158</v>
-      </c>
-      <c r="D45" s="20">
-        <f>SUM(D4:D44)</f>
-        <v>1421702</v>
-      </c>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="35" t="s">
+      <c r="C46" s="20">
+        <f>SUM(C4:C45)</f>
+        <v>33708381</v>
+      </c>
+      <c r="D46" s="20">
+        <f>SUM(D4:D45)</f>
+        <v>1612012</v>
+      </c>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B47" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="B47:F47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2203,23 +2272,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:E43"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>7</v>
       </c>
@@ -2236,7 +2305,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
@@ -2253,7 +2322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="32" t="s">
         <v>11</v>
       </c>
@@ -2270,7 +2339,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
         <v>12</v>
       </c>
@@ -2287,7 +2356,7 @@
         <v>185655.005</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -2304,7 +2373,7 @@
         <v>284580.19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
         <v>14</v>
       </c>
@@ -2321,7 +2390,7 @@
         <v>462880.00530000002</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
         <v>15</v>
       </c>
@@ -2338,7 +2407,7 @@
         <v>596910.04500000004</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="32" t="s">
         <v>16</v>
       </c>
@@ -2355,7 +2424,7 @@
         <v>580890</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
         <v>17</v>
       </c>
@@ -2372,7 +2441,7 @@
         <v>741399</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
         <v>18</v>
       </c>
@@ -2389,7 +2458,7 @@
         <v>820491</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
         <v>19</v>
       </c>
@@ -2406,7 +2475,7 @@
         <v>831816.00349999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="32" t="s">
         <v>20</v>
       </c>
@@ -2423,7 +2492,7 @@
         <v>874362</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="32" t="s">
         <v>21</v>
       </c>
@@ -2440,7 +2509,7 @@
         <v>888561</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
         <v>22</v>
       </c>
@@ -2457,7 +2526,7 @@
         <v>896041</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="32" t="s">
         <v>23</v>
       </c>
@@ -2474,7 +2543,7 @@
         <v>939801</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="32" t="s">
         <v>24</v>
       </c>
@@ -2491,7 +2560,7 @@
         <v>974698</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="32" t="s">
         <v>25</v>
       </c>
@@ -2508,7 +2577,7 @@
         <v>1010309</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="32" t="s">
         <v>26</v>
       </c>
@@ -2525,7 +2594,7 @@
         <v>994060</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="32" t="s">
         <v>27</v>
       </c>
@@ -2542,7 +2611,7 @@
         <v>1003758</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="32" t="s">
         <v>28</v>
       </c>
@@ -2559,7 +2628,7 @@
         <v>1020962</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="32" t="s">
         <v>29</v>
       </c>
@@ -2576,7 +2645,7 @@
         <v>1041871.025</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="32" t="s">
         <v>30</v>
       </c>
@@ -2593,7 +2662,7 @@
         <v>1063581</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>31</v>
       </c>
@@ -2610,7 +2679,7 @@
         <v>1063790</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
         <v>32</v>
       </c>
@@ -2627,7 +2696,7 @@
         <v>1048585</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
         <v>33</v>
       </c>
@@ -2644,7 +2713,7 @@
         <v>1153170</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
         <v>34</v>
       </c>
@@ -2661,7 +2730,7 @@
         <v>1306192</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="28" t="s">
         <v>35</v>
       </c>
@@ -2678,7 +2747,7 @@
         <v>1155779</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
         <v>36</v>
       </c>
@@ -2695,7 +2764,7 @@
         <v>1154136.69</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
         <v>37</v>
       </c>
@@ -2712,7 +2781,7 @@
         <v>1217216</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="29" t="s">
         <v>38</v>
       </c>
@@ -2729,7 +2798,7 @@
         <v>1339112</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="29" t="s">
         <v>39</v>
       </c>
@@ -2746,7 +2815,7 @@
         <v>1354917</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="29" t="s">
         <v>40</v>
       </c>
@@ -2763,7 +2832,7 @@
         <v>1457887</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="29" t="s">
         <v>41</v>
       </c>
@@ -2780,7 +2849,7 @@
         <v>1568002</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="29" t="s">
         <v>49</v>
       </c>
@@ -2797,7 +2866,7 @@
         <v>1606830</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="29" t="s">
         <v>50</v>
       </c>
@@ -2814,7 +2883,7 @@
         <v>1612826</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="29" t="s">
         <v>51</v>
       </c>
@@ -2831,7 +2900,7 @@
         <v>1596042</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="29" t="s">
         <v>52</v>
       </c>
@@ -2848,7 +2917,7 @@
         <v>1677221</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="29" t="s">
         <v>53</v>
       </c>
@@ -2865,7 +2934,7 @@
         <v>1812210</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="29" t="s">
         <v>56</v>
       </c>
@@ -2882,7 +2951,7 @@
         <v>1837984</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="29" t="s">
         <v>58</v>
       </c>
@@ -2899,7 +2968,7 @@
         <v>1918794</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="29" t="s">
         <v>61</v>
       </c>
@@ -2916,7 +2985,7 @@
         <v>1944190</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="29" t="s">
         <v>64</v>
       </c>
@@ -2931,6 +3000,23 @@
       </c>
       <c r="E43" s="33">
         <v>2019604</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="29">
+        <v>181</v>
+      </c>
+      <c r="C44" s="33">
+        <v>204862.4</v>
+      </c>
+      <c r="D44" s="33">
+        <v>1364843.28</v>
+      </c>
+      <c r="E44" s="33">
+        <v>1203720.93</v>
       </c>
     </row>
   </sheetData>
@@ -2940,21 +3026,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:C37"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -2966,7 +3052,7 @@
       </c>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>25</v>
       </c>
@@ -2978,7 +3064,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>34</v>
       </c>
@@ -2990,7 +3076,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>29</v>
       </c>
@@ -3002,7 +3088,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>30</v>
       </c>
@@ -3014,7 +3100,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>29</v>
       </c>
@@ -3026,7 +3112,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>27</v>
       </c>
@@ -3038,7 +3124,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>28</v>
       </c>
@@ -3050,7 +3136,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>24</v>
       </c>
@@ -3062,7 +3148,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>28</v>
       </c>
@@ -3074,7 +3160,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>51</v>
       </c>
@@ -3086,7 +3172,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>46</v>
       </c>
@@ -3098,7 +3184,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>71</v>
       </c>
@@ -3110,7 +3196,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>46</v>
       </c>
@@ -3122,7 +3208,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>25</v>
       </c>
@@ -3134,7 +3220,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>42</v>
       </c>
@@ -3146,7 +3232,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>22</v>
       </c>
@@ -3158,7 +3244,7 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>24</v>
       </c>
@@ -3170,7 +3256,7 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>36</v>
       </c>
@@ -3182,7 +3268,7 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>44</v>
       </c>
@@ -3194,7 +3280,7 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>49</v>
       </c>
@@ -3206,7 +3292,7 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>49</v>
       </c>
@@ -3218,7 +3304,7 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>48</v>
       </c>
@@ -3230,7 +3316,7 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>51</v>
       </c>
@@ -3242,7 +3328,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>43</v>
       </c>
@@ -3253,7 +3339,7 @@
         <v>12876</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>46</v>
       </c>
@@ -3264,7 +3350,7 @@
         <v>15983</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>42</v>
       </c>
@@ -3275,7 +3361,7 @@
         <v>8245.0000999999993</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>47</v>
       </c>
@@ -3286,7 +3372,7 @@
         <v>16840</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="32">
         <v>52</v>
       </c>
@@ -3297,7 +3383,7 @@
         <v>20799</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="32">
         <v>57</v>
       </c>
@@ -3308,7 +3394,7 @@
         <v>68574</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="32">
         <v>69</v>
       </c>
@@ -3319,7 +3405,7 @@
         <v>98931</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="32">
         <v>66</v>
       </c>
@@ -3330,7 +3416,7 @@
         <v>60113</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="32">
         <v>58</v>
       </c>
@@ -3341,7 +3427,7 @@
         <v>23654</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="32">
         <v>48</v>
       </c>
@@ -3352,7 +3438,7 @@
         <v>17037</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="32">
         <v>53</v>
       </c>
@@ -3363,7 +3449,7 @@
         <v>14091</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="32">
         <v>50</v>
       </c>
@@ -3374,7 +3460,7 @@
         <v>12237</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="28">
         <v>50</v>
       </c>
@@ -3383,6 +3469,17 @@
       </c>
       <c r="C37" s="33">
         <v>19009</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="28">
+        <v>57</v>
+      </c>
+      <c r="B38" s="28">
+        <v>51</v>
+      </c>
+      <c r="C38" s="33">
+        <v>21364.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add RKI data downloaded 2021-01-15--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Testzahlen-gesamt.xlsx
+++ b/rki-data/RKI-Testzahlen-gesamt.xlsx
@@ -4,9 +4,9 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20368"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D5A673F-047C-4ED6-87C2-F21DD996B5CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72A8C6D-CF96-47E2-BA0C-1E469381DEE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="3810" windowWidth="19440" windowHeight="11040" tabRatio="301" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="3810" windowWidth="19440" windowHeight="11040" tabRatio="301" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterungen" sheetId="5" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
-  <si>
-    <t>Kalenderwoche 2020</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t>Anzahl Testungen</t>
   </si>
@@ -30,9 +27,6 @@
     <t>Positiv getestet</t>
   </si>
   <si>
-    <t>Bis einschließlich KW10</t>
-  </si>
-  <si>
     <t>Anzahl übermittelnde Labore</t>
   </si>
   <si>
@@ -72,36 +66,12 @@
     <t xml:space="preserve">Zusätzlich zur Anzahl durchgeführter Tests werden in der RKI-Testlaborabfrage und durch einen labormedizinischen Berufsverband Angaben zur täglichen (aktuellen) Testkapazität, zur Reichweite sowie zu möglichen Probenrückstaus befragt. Die Reichweite gibt an, wie viele Arbeitstage ein Labor unter Vollauslastung  der angegebenen maximalen Testkapazität unter Berücksichtigung aller notwendigen Ressourcen (Entnahmematerial, Testreagenzien, Personal u. a.) zum Zeitpunkt der Abfrage arbeiten kann. Da die Reichweite stark  vom Vorhandensein von Testreagenzien abhängig ist, stellt die Angabe eine Momentaufnahme in einem dynamischen System dar (s. Testzkapazitäten, Probenrückstau). </t>
   </si>
   <si>
-    <t>46*</t>
-  </si>
-  <si>
-    <t>47*</t>
-  </si>
-  <si>
-    <t>48*</t>
-  </si>
-  <si>
     <t>*Ab 03. November 2020 geänderte Testkriterien, Daten nicht direkt mit Vorwochen vergleichbar</t>
   </si>
   <si>
-    <t>49*</t>
-  </si>
-  <si>
     <t>Bisher haben sich mehr als 250 Labore für die RKI-Testlaborabfrage oder in einem der anderen übermittelnden Netzwerke registriert und übermitteln nach Aufruf überwiegend wöchentlich. Da Labore in der RKI-Testzahlabfrage  die  Tests  der  vergangenen Kalenderwochen nachmelden bzw. korrigieren können, ist es möglich, dass sich die ermittelten Zahlen nachträglich ändern. Es ist zu beachten, dass die Zahl der Tests nicht mit der Zahl der getesteten Personen gleichzusetzen ist, da in den Angaben Mehrfachtestungen von Patienten enthalten sein können (s. Testzahlen).</t>
   </si>
   <si>
-    <t>50*</t>
-  </si>
-  <si>
-    <t>51*</t>
-  </si>
-  <si>
-    <t>52*</t>
-  </si>
-  <si>
-    <t>53*</t>
-  </si>
-  <si>
     <t>2020, KW11</t>
   </si>
   <si>
@@ -232,6 +202,147 @@
   </si>
   <si>
     <t>2021, KW1</t>
+  </si>
+  <si>
+    <t>Kalenderwoche</t>
+  </si>
+  <si>
+    <t>Bis einschließlich KW10, 2020</t>
+  </si>
+  <si>
+    <t>11/2020</t>
+  </si>
+  <si>
+    <t>12/2020</t>
+  </si>
+  <si>
+    <t>13/2020</t>
+  </si>
+  <si>
+    <t>14/2020</t>
+  </si>
+  <si>
+    <t>15/2020</t>
+  </si>
+  <si>
+    <t>16/2020</t>
+  </si>
+  <si>
+    <t>17/2020</t>
+  </si>
+  <si>
+    <t>18/2020</t>
+  </si>
+  <si>
+    <t>19/2020</t>
+  </si>
+  <si>
+    <t>20/2020</t>
+  </si>
+  <si>
+    <t>21/2020</t>
+  </si>
+  <si>
+    <t>22/2020</t>
+  </si>
+  <si>
+    <t>23/2020</t>
+  </si>
+  <si>
+    <t>24/2020</t>
+  </si>
+  <si>
+    <t>25/2020</t>
+  </si>
+  <si>
+    <t>26/2020</t>
+  </si>
+  <si>
+    <t>27/2020</t>
+  </si>
+  <si>
+    <t>28/2020</t>
+  </si>
+  <si>
+    <t>29/2020</t>
+  </si>
+  <si>
+    <t>30/2020</t>
+  </si>
+  <si>
+    <t>31/2020</t>
+  </si>
+  <si>
+    <t>32/2020</t>
+  </si>
+  <si>
+    <t>33/2020</t>
+  </si>
+  <si>
+    <t>34/2020</t>
+  </si>
+  <si>
+    <t>35/2020</t>
+  </si>
+  <si>
+    <t>36/2020</t>
+  </si>
+  <si>
+    <t>37/2020</t>
+  </si>
+  <si>
+    <t>38/2020</t>
+  </si>
+  <si>
+    <t>39/2020</t>
+  </si>
+  <si>
+    <t>40/2020</t>
+  </si>
+  <si>
+    <t>41/2020</t>
+  </si>
+  <si>
+    <t>42/2020</t>
+  </si>
+  <si>
+    <t>43/2020</t>
+  </si>
+  <si>
+    <t>44/2020</t>
+  </si>
+  <si>
+    <t>45/2020</t>
+  </si>
+  <si>
+    <t>46/2020*</t>
+  </si>
+  <si>
+    <t>47/2020*</t>
+  </si>
+  <si>
+    <t>48/2020*</t>
+  </si>
+  <si>
+    <t>49/2020*</t>
+  </si>
+  <si>
+    <t>50/2020*</t>
+  </si>
+  <si>
+    <t>51/2020*</t>
+  </si>
+  <si>
+    <t>52/2020*</t>
+  </si>
+  <si>
+    <t>53/2020*</t>
+  </si>
+  <si>
+    <t>1/2021*</t>
+  </si>
+  <si>
+    <t>2021, KW2</t>
   </si>
 </sst>
 </file>
@@ -391,7 +502,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -494,6 +605,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Comma" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -591,9 +705,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Probenrückstau!$A$2:$B$40</c:f>
+              <c:f>Probenrückstau!$A$2:$B$41</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>15</c:v>
@@ -711,6 +825,9 @@
                   </c:pt>
                   <c:pt idx="38">
                     <c:v>53</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>1</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -830,6 +947,9 @@
                   </c:pt>
                   <c:pt idx="38">
                     <c:v>40</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>47</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -837,10 +957,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Probenrückstau!$C$2:$C$40</c:f>
+              <c:f>Probenrückstau!$C$2:$C$41</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>3423</c:v>
                 </c:pt>
@@ -957,6 +1077,9 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>6557</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11691.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,7 +1571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1459,17 +1582,17 @@
   <sheetData>
     <row r="3" spans="1:1" s="1" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="126" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1480,10 +1603,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:F49"/>
+  <dimension ref="B3:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1496,24 +1619,24 @@
   <sheetData>
     <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>2</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="C4" s="12">
         <v>124716</v>
@@ -1530,8 +1653,8 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="11">
-        <v>11</v>
+      <c r="B5" s="36" t="s">
+        <v>63</v>
       </c>
       <c r="C5" s="12">
         <v>127457</v>
@@ -1548,8 +1671,8 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="11">
-        <v>12</v>
+      <c r="B6" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="C6" s="12">
         <v>348619</v>
@@ -1566,8 +1689,8 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="13">
-        <v>13</v>
+      <c r="B7" s="36" t="s">
+        <v>65</v>
       </c>
       <c r="C7" s="15">
         <v>361515</v>
@@ -1584,8 +1707,8 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="19">
-        <v>14</v>
+      <c r="B8" s="36" t="s">
+        <v>66</v>
       </c>
       <c r="C8" s="14">
         <v>408348</v>
@@ -1602,8 +1725,8 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="19">
-        <v>15</v>
+      <c r="B9" s="36" t="s">
+        <v>67</v>
       </c>
       <c r="C9" s="16">
         <v>380197</v>
@@ -1620,8 +1743,8 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="19">
-        <v>16</v>
+      <c r="B10" s="36" t="s">
+        <v>68</v>
       </c>
       <c r="C10" s="16">
         <v>331902</v>
@@ -1638,8 +1761,8 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="17">
-        <v>17</v>
+      <c r="B11" s="36" t="s">
+        <v>69</v>
       </c>
       <c r="C11" s="16">
         <v>363890</v>
@@ -1656,8 +1779,8 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="17">
-        <v>18</v>
+      <c r="B12" s="36" t="s">
+        <v>70</v>
       </c>
       <c r="C12" s="18">
         <v>326788</v>
@@ -1674,8 +1797,8 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="17">
-        <v>19</v>
+      <c r="B13" s="36" t="s">
+        <v>71</v>
       </c>
       <c r="C13" s="18">
         <v>403875</v>
@@ -1692,8 +1815,8 @@
       </c>
     </row>
     <row r="14" spans="2:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="17">
-        <v>20</v>
+      <c r="B14" s="36" t="s">
+        <v>72</v>
       </c>
       <c r="C14" s="18">
         <v>431146</v>
@@ -1702,7 +1825,7 @@
         <v>7069</v>
       </c>
       <c r="E14" s="22">
-        <f t="shared" ref="E14:E47" si="1">(D14/C14)*100</f>
+        <f t="shared" ref="E14:E48" si="1">(D14/C14)*100</f>
         <v>1.6395838068774846</v>
       </c>
       <c r="F14" s="17">
@@ -1710,8 +1833,8 @@
       </c>
     </row>
     <row r="15" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="17">
-        <v>21</v>
+      <c r="B15" s="36" t="s">
+        <v>73</v>
       </c>
       <c r="C15" s="18">
         <v>354260</v>
@@ -1728,8 +1851,8 @@
       </c>
     </row>
     <row r="16" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="17">
-        <v>22</v>
+      <c r="B16" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="C16" s="18">
         <v>401589</v>
@@ -1746,8 +1869,8 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B17" s="17">
-        <v>23</v>
+      <c r="B17" s="36" t="s">
+        <v>75</v>
       </c>
       <c r="C17" s="18">
         <v>337217</v>
@@ -1764,8 +1887,8 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="17">
-        <v>24</v>
+      <c r="B18" s="36" t="s">
+        <v>76</v>
       </c>
       <c r="C18" s="18">
         <v>327196</v>
@@ -1782,8 +1905,8 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="17">
-        <v>25</v>
+      <c r="B19" s="36" t="s">
+        <v>77</v>
       </c>
       <c r="C19" s="18">
         <v>381933</v>
@@ -1800,8 +1923,8 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="17">
-        <v>26</v>
+      <c r="B20" s="36" t="s">
+        <v>78</v>
       </c>
       <c r="C20" s="18">
         <v>464626</v>
@@ -1818,8 +1941,8 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="17">
-        <v>27</v>
+      <c r="B21" s="36" t="s">
+        <v>79</v>
       </c>
       <c r="C21" s="18">
         <v>506459</v>
@@ -1836,8 +1959,8 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="17">
-        <v>28</v>
+      <c r="B22" s="36" t="s">
+        <v>80</v>
       </c>
       <c r="C22" s="18">
         <v>510551</v>
@@ -1854,8 +1977,8 @@
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="17">
-        <v>29</v>
+      <c r="B23" s="36" t="s">
+        <v>81</v>
       </c>
       <c r="C23" s="18">
         <v>538701</v>
@@ -1872,8 +1995,8 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="17">
-        <v>30</v>
+      <c r="B24" s="36" t="s">
+        <v>82</v>
       </c>
       <c r="C24" s="18">
         <v>553742</v>
@@ -1890,8 +2013,8 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="17">
-        <v>31</v>
+      <c r="B25" s="36" t="s">
+        <v>83</v>
       </c>
       <c r="C25" s="18">
         <v>586967</v>
@@ -1908,8 +2031,8 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="17">
-        <v>32</v>
+      <c r="B26" s="36" t="s">
+        <v>84</v>
       </c>
       <c r="C26" s="18">
         <v>717123</v>
@@ -1926,8 +2049,8 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="17">
-        <v>33</v>
+      <c r="B27" s="36" t="s">
+        <v>85</v>
       </c>
       <c r="C27" s="18">
         <v>835384</v>
@@ -1944,8 +2067,8 @@
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="17">
-        <v>34</v>
+      <c r="B28" s="36" t="s">
+        <v>86</v>
       </c>
       <c r="C28" s="18">
         <v>1029715</v>
@@ -1962,8 +2085,8 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="17">
-        <v>35</v>
+      <c r="B29" s="36" t="s">
+        <v>87</v>
       </c>
       <c r="C29" s="18">
         <v>1091207</v>
@@ -1980,8 +2103,8 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="17">
-        <v>36</v>
+      <c r="B30" s="36" t="s">
+        <v>88</v>
       </c>
       <c r="C30" s="18">
         <v>1043713</v>
@@ -1998,8 +2121,8 @@
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="17">
-        <v>37</v>
+      <c r="B31" s="36" t="s">
+        <v>89</v>
       </c>
       <c r="C31" s="18">
         <v>1133737</v>
@@ -2016,8 +2139,8 @@
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B32" s="17">
-        <v>38</v>
+      <c r="B32" s="36" t="s">
+        <v>90</v>
       </c>
       <c r="C32" s="18">
         <v>1090740</v>
@@ -2034,8 +2157,8 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B33" s="17">
-        <v>39</v>
+      <c r="B33" s="36" t="s">
+        <v>91</v>
       </c>
       <c r="C33" s="18">
         <v>1154700</v>
@@ -2052,8 +2175,8 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B34" s="17">
-        <v>40</v>
+      <c r="B34" s="36" t="s">
+        <v>92</v>
       </c>
       <c r="C34" s="18">
         <v>1112967</v>
@@ -2070,8 +2193,8 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B35" s="17">
-        <v>41</v>
+      <c r="B35" s="36" t="s">
+        <v>93</v>
       </c>
       <c r="C35" s="18">
         <v>1188338</v>
@@ -2088,8 +2211,8 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B36" s="17">
-        <v>42</v>
+      <c r="B36" s="36" t="s">
+        <v>94</v>
       </c>
       <c r="C36" s="18">
         <v>1220909</v>
@@ -2106,8 +2229,8 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B37" s="17">
-        <v>43</v>
+      <c r="B37" s="36" t="s">
+        <v>95</v>
       </c>
       <c r="C37" s="18">
         <v>1373753</v>
@@ -2124,8 +2247,8 @@
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B38" s="17">
-        <v>44</v>
+      <c r="B38" s="36" t="s">
+        <v>96</v>
       </c>
       <c r="C38" s="18">
         <v>1593278</v>
@@ -2142,8 +2265,8 @@
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B39" s="17">
-        <v>45</v>
+      <c r="B39" s="36" t="s">
+        <v>97</v>
       </c>
       <c r="C39" s="18">
         <v>1598527</v>
@@ -2160,8 +2283,8 @@
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B40" s="17" t="s">
-        <v>17</v>
+      <c r="B40" s="36" t="s">
+        <v>98</v>
       </c>
       <c r="C40" s="18">
         <v>1396088</v>
@@ -2178,8 +2301,8 @@
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B41" s="17" t="s">
-        <v>18</v>
+      <c r="B41" s="36" t="s">
+        <v>99</v>
       </c>
       <c r="C41" s="18">
         <v>1367570</v>
@@ -2196,8 +2319,8 @@
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B42" s="17" t="s">
-        <v>19</v>
+      <c r="B42" s="36" t="s">
+        <v>100</v>
       </c>
       <c r="C42" s="18">
         <v>1353980</v>
@@ -2214,8 +2337,8 @@
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B43" s="17" t="s">
-        <v>21</v>
+      <c r="B43" s="36" t="s">
+        <v>101</v>
       </c>
       <c r="C43" s="18">
         <v>1329716</v>
@@ -2232,26 +2355,26 @@
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B44" s="17" t="s">
-        <v>23</v>
+      <c r="B44" s="36" t="s">
+        <v>102</v>
       </c>
       <c r="C44" s="18">
-        <v>1442099</v>
+        <v>1445671</v>
       </c>
       <c r="D44" s="18">
-        <v>165516</v>
+        <v>165953</v>
       </c>
       <c r="E44" s="22">
         <f t="shared" si="1"/>
-        <v>11.477436708575487</v>
+        <v>11.479306149186087</v>
       </c>
       <c r="F44" s="17">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B45" s="17" t="s">
-        <v>24</v>
+      <c r="B45" s="36" t="s">
+        <v>103</v>
       </c>
       <c r="C45" s="18">
         <v>1612673</v>
@@ -2268,69 +2391,87 @@
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B46" s="17" t="s">
-        <v>25</v>
+      <c r="B46" s="36" t="s">
+        <v>104</v>
       </c>
       <c r="C46" s="18">
-        <v>1071001</v>
+        <v>1076581</v>
       </c>
       <c r="D46" s="18">
-        <v>138338</v>
+        <v>138751</v>
       </c>
       <c r="E46" s="22">
         <f t="shared" si="1"/>
-        <v>12.916701291595434</v>
+        <v>12.888115246321458</v>
       </c>
       <c r="F46" s="17">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B47" s="17" t="s">
-        <v>26</v>
+      <c r="B47" s="36" t="s">
+        <v>105</v>
       </c>
       <c r="C47" s="18">
-        <v>789680</v>
+        <v>804617</v>
       </c>
       <c r="D47" s="18">
-        <v>126884</v>
+        <v>127805</v>
       </c>
       <c r="E47" s="22">
         <f t="shared" si="1"/>
-        <v>16.06777428831932</v>
+        <v>15.883954726285923</v>
       </c>
       <c r="F47" s="17">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B48" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="20">
-        <f>SUM(C4:C47)</f>
-        <v>35118592</v>
-      </c>
-      <c r="D48" s="20">
-        <f>SUM(D4:D47)</f>
-        <v>1866295</v>
-      </c>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
+      <c r="B48" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="18">
+        <v>1210515</v>
+      </c>
+      <c r="D48" s="18">
+        <v>154709</v>
+      </c>
+      <c r="E48" s="22">
+        <f t="shared" si="1"/>
+        <v>12.780428164871976</v>
+      </c>
+      <c r="F48" s="17">
+        <v>193</v>
+      </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B49" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
+      <c r="B49" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="20">
+        <f>SUM(C4:C48)</f>
+        <v>36353196</v>
+      </c>
+      <c r="D49" s="20">
+        <f>SUM(D4:D48)</f>
+        <v>2022775</v>
+      </c>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B50" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="B50:F50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2339,10 +2480,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:E46"/>
+  <dimension ref="A2:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2356,24 +2497,24 @@
   <sheetData>
     <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B3" s="24">
         <v>28</v>
@@ -2382,15 +2523,15 @@
         <v>7115</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="32" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B4" s="24">
         <v>93</v>
@@ -2399,15 +2540,15 @@
         <v>31010</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B5" s="24">
         <v>111</v>
@@ -2416,7 +2557,7 @@
         <v>64725</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" s="33">
         <v>185655.005</v>
@@ -2424,7 +2565,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B6" s="24">
         <v>113</v>
@@ -2433,7 +2574,7 @@
         <v>103515</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E6" s="33">
         <v>284580.19</v>
@@ -2441,7 +2582,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B7" s="24">
         <v>132</v>
@@ -2450,7 +2591,7 @@
         <v>116655</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7" s="33">
         <v>462880.00530000002</v>
@@ -2458,7 +2599,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B8" s="24">
         <v>112</v>
@@ -2475,7 +2616,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="32" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B9" s="24">
         <v>126</v>
@@ -2492,7 +2633,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B10" s="24">
         <v>133</v>
@@ -2509,7 +2650,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B11" s="24">
         <v>137</v>
@@ -2526,7 +2667,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B12" s="24">
         <v>134</v>
@@ -2543,7 +2684,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="32" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B13" s="32">
         <v>136</v>
@@ -2560,7 +2701,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="32" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B14" s="32">
         <v>143</v>
@@ -2577,7 +2718,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B15" s="32">
         <v>137</v>
@@ -2594,7 +2735,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="32" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B16" s="32">
         <v>139</v>
@@ -2611,7 +2752,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="32" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B17" s="32">
         <v>138</v>
@@ -2628,7 +2769,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="32" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B18" s="32">
         <v>137</v>
@@ -2645,7 +2786,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="32" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B19" s="32">
         <v>137</v>
@@ -2662,7 +2803,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="32" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B20" s="32">
         <v>145</v>
@@ -2679,7 +2820,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="32" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B21" s="32">
         <v>146</v>
@@ -2696,7 +2837,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="32" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B22" s="32">
         <v>145</v>
@@ -2713,7 +2854,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="32" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B23" s="32">
         <v>145</v>
@@ -2730,7 +2871,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="32" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B24" s="26">
         <v>149</v>
@@ -2747,7 +2888,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="32" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B25" s="26">
         <v>151</v>
@@ -2764,7 +2905,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="32" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B26" s="26">
         <v>157</v>
@@ -2781,7 +2922,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="32" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B27" s="26">
         <v>163</v>
@@ -2798,7 +2939,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="32" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B28" s="26">
         <v>168</v>
@@ -2815,7 +2956,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="32" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B29" s="26">
         <v>168</v>
@@ -2832,7 +2973,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="32" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B30" s="29">
         <v>165</v>
@@ -2849,7 +2990,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="32" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B31" s="29">
         <v>170</v>
@@ -2866,7 +3007,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B32" s="29">
         <v>168</v>
@@ -2883,7 +3024,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="32" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B33" s="29">
         <v>166</v>
@@ -2900,7 +3041,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="32" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B34" s="29">
         <v>164</v>
@@ -2917,7 +3058,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="32" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B35" s="29">
         <v>167</v>
@@ -2934,7 +3075,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="32" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B36" s="29">
         <v>184</v>
@@ -2951,7 +3092,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="32" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B37" s="29">
         <v>176</v>
@@ -2968,7 +3109,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="32" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B38" s="29">
         <v>170</v>
@@ -2985,7 +3126,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="32" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B39" s="29">
         <v>175</v>
@@ -3002,7 +3143,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="32" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B40" s="29">
         <v>169</v>
@@ -3019,7 +3160,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="32" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B41" s="29">
         <v>168</v>
@@ -3036,7 +3177,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="32" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B42" s="29">
         <v>175</v>
@@ -3053,7 +3194,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="32" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B43" s="29">
         <v>175</v>
@@ -3070,7 +3211,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="32" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B44" s="29">
         <v>181</v>
@@ -3087,7 +3228,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="32" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B45" s="29">
         <v>173</v>
@@ -3104,7 +3245,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="29" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B46" s="29">
         <v>177</v>
@@ -3117,6 +3258,23 @@
       </c>
       <c r="E46" s="33">
         <v>1874827</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="29">
+        <v>176</v>
+      </c>
+      <c r="C47" s="33">
+        <v>334756</v>
+      </c>
+      <c r="D47" s="33">
+        <v>2222744</v>
+      </c>
+      <c r="E47" s="33">
+        <v>2017760</v>
       </c>
     </row>
   </sheetData>
@@ -3127,9 +3285,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -3142,13 +3300,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="D1" s="6"/>
     </row>
@@ -3602,6 +3760,17 @@
       </c>
       <c r="C40" s="33">
         <v>6557</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="28">
+        <v>47</v>
+      </c>
+      <c r="B41" s="28">
+        <v>1</v>
+      </c>
+      <c r="C41" s="33">
+        <v>11691.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add RKI data downloaded 2021-02-04--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Testzahlen-gesamt.xlsx
+++ b/rki-data/RKI-Testzahlen-gesamt.xlsx
@@ -4,9 +4,9 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20368"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE04D2E-F096-4D90-A359-229E598B3514}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CA3B57-5D52-4310-9D00-198FAB0DF76A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="5610" windowWidth="19440" windowHeight="11040" tabRatio="301" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="6810" windowWidth="19440" windowHeight="11040" tabRatio="301" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterungen" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="114">
   <si>
     <t>Anzahl Testungen</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>2021, KW4</t>
+  </si>
+  <si>
+    <t>4/2021*</t>
+  </si>
+  <si>
+    <t>2021, KW 5</t>
   </si>
 </sst>
 </file>
@@ -702,9 +708,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Probenrückstau!$A$2:$B$43</c:f>
+              <c:f>Probenrückstau!$A$2:$B$44</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>15</c:v>
@@ -831,6 +837,9 @@
                   </c:pt>
                   <c:pt idx="41">
                     <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="42">
+                    <c:v>4</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -959,6 +968,9 @@
                   </c:pt>
                   <c:pt idx="41">
                     <c:v>48</c:v>
+                  </c:pt>
+                  <c:pt idx="42">
+                    <c:v>42</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -966,10 +978,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Probenrückstau!$C$2:$C$43</c:f>
+              <c:f>Probenrückstau!$C$2:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>3423</c:v>
                 </c:pt>
@@ -1095,6 +1107,9 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>11980</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1618,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:F52"/>
+  <dimension ref="B3:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,35 +1669,29 @@
         <v>62</v>
       </c>
       <c r="C4" s="12">
-        <v>62253</v>
+        <v>64388</v>
       </c>
       <c r="D4" s="12">
-        <v>1589</v>
-      </c>
-      <c r="E4" s="16">
-        <f>(D4/C4)*100</f>
-        <v>2.5524874303246432</v>
-      </c>
-      <c r="F4" s="11">
-        <v>90</v>
-      </c>
+        <v>1634</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="12">
-        <v>126890</v>
+        <v>127750</v>
       </c>
       <c r="D5" s="12">
-        <v>7419</v>
+        <v>7456</v>
       </c>
       <c r="E5" s="16">
-        <f t="shared" ref="E5:E50" si="0">(D5/C5)*100</f>
-        <v>5.8467964378595632</v>
+        <v>5.8363992172211354</v>
       </c>
       <c r="F5" s="11">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1690,17 +1699,16 @@
         <v>64</v>
       </c>
       <c r="C6" s="12">
-        <v>368346</v>
+        <v>373856</v>
       </c>
       <c r="D6" s="12">
-        <v>25205</v>
+        <v>25847</v>
       </c>
       <c r="E6" s="16">
-        <f t="shared" si="0"/>
-        <v>6.8427511090116351</v>
+        <v>6.9136244971325853</v>
       </c>
       <c r="F6" s="11">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1708,17 +1716,16 @@
         <v>65</v>
       </c>
       <c r="C7" s="12">
-        <v>369781</v>
+        <v>376920</v>
       </c>
       <c r="D7" s="12">
-        <v>32158</v>
+        <v>33045</v>
       </c>
       <c r="E7" s="16">
-        <f t="shared" si="0"/>
-        <v>8.6964987384424841</v>
+        <v>8.7671123845908951</v>
       </c>
       <c r="F7" s="11">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1726,17 +1733,16 @@
         <v>66</v>
       </c>
       <c r="C8" s="12">
-        <v>409201</v>
+        <v>416510</v>
       </c>
       <c r="D8" s="12">
-        <v>36885</v>
+        <v>37591</v>
       </c>
       <c r="E8" s="16">
-        <f t="shared" si="0"/>
-        <v>9.013907590646161</v>
+        <v>9.0252334877914091</v>
       </c>
       <c r="F8" s="11">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1744,17 +1750,16 @@
         <v>67</v>
       </c>
       <c r="C9" s="12">
-        <v>372846</v>
+        <v>386165</v>
       </c>
       <c r="D9" s="12">
-        <v>29552</v>
+        <v>30812</v>
       </c>
       <c r="E9" s="16">
-        <f t="shared" si="0"/>
-        <v>7.9260606255665875</v>
+        <v>7.9789727189154895</v>
       </c>
       <c r="F9" s="11">
-        <v>164</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1762,17 +1767,16 @@
         <v>68</v>
       </c>
       <c r="C10" s="12">
-        <v>337590</v>
+        <v>339983</v>
       </c>
       <c r="D10" s="12">
-        <v>22616</v>
+        <v>22724</v>
       </c>
       <c r="E10" s="16">
-        <f t="shared" si="0"/>
-        <v>6.6992505702183127</v>
+        <v>6.6838636049449534</v>
       </c>
       <c r="F10" s="11">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1780,14 +1784,13 @@
         <v>69</v>
       </c>
       <c r="C11" s="12">
-        <v>362741</v>
+        <v>363659</v>
       </c>
       <c r="D11" s="12">
-        <v>18101</v>
+        <v>18127</v>
       </c>
       <c r="E11" s="16">
-        <f t="shared" si="0"/>
-        <v>4.9900617796168616</v>
+        <v>4.984614707734444</v>
       </c>
       <c r="F11" s="11">
         <v>180</v>
@@ -1798,17 +1801,16 @@
         <v>70</v>
       </c>
       <c r="C12" s="12">
-        <v>326270</v>
+        <v>327799</v>
       </c>
       <c r="D12" s="12">
-        <v>12577</v>
+        <v>12600</v>
       </c>
       <c r="E12" s="16">
-        <f t="shared" si="0"/>
-        <v>3.8547828485610078</v>
+        <v>3.8438189256221036</v>
       </c>
       <c r="F12" s="11">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -1816,17 +1818,16 @@
         <v>71</v>
       </c>
       <c r="C13" s="12">
-        <v>383807</v>
+        <v>385638</v>
       </c>
       <c r="D13" s="12">
-        <v>10172</v>
+        <v>10181</v>
       </c>
       <c r="E13" s="16">
-        <f t="shared" si="0"/>
-        <v>2.6502903803213593</v>
+        <v>2.6400406598934754</v>
       </c>
       <c r="F13" s="11">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="2:6" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1834,17 +1835,16 @@
         <v>72</v>
       </c>
       <c r="C14" s="12">
-        <v>431145</v>
+        <v>431682</v>
       </c>
       <c r="D14" s="12">
-        <v>7069</v>
+        <v>7142</v>
       </c>
       <c r="E14" s="16">
-        <f t="shared" si="0"/>
-        <v>1.6395876097368633</v>
+        <v>1.6544586061035669</v>
       </c>
       <c r="F14" s="11">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1852,17 +1852,16 @@
         <v>73</v>
       </c>
       <c r="C15" s="12">
-        <v>354260</v>
+        <v>356489</v>
       </c>
       <c r="D15" s="12">
-        <v>5228</v>
+        <v>5315</v>
       </c>
       <c r="E15" s="16">
-        <f t="shared" si="0"/>
-        <v>1.4757522723423475</v>
+        <v>1.4909295939005129</v>
       </c>
       <c r="F15" s="11">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1870,17 +1869,16 @@
         <v>74</v>
       </c>
       <c r="C16" s="12">
-        <v>401589</v>
+        <v>408078</v>
       </c>
       <c r="D16" s="12">
-        <v>4267</v>
+        <v>4335</v>
       </c>
       <c r="E16" s="16">
-        <f t="shared" si="0"/>
-        <v>1.0625291031377853</v>
+        <v>1.0622969138252982</v>
       </c>
       <c r="F16" s="11">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1888,17 +1886,16 @@
         <v>75</v>
       </c>
       <c r="C17" s="12">
-        <v>337217</v>
+        <v>342328</v>
       </c>
       <c r="D17" s="12">
-        <v>3085</v>
+        <v>3219</v>
       </c>
       <c r="E17" s="16">
-        <f t="shared" si="0"/>
-        <v>0.9148411853494931</v>
+        <v>0.94032623682550076</v>
       </c>
       <c r="F17" s="11">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -1906,17 +1903,16 @@
         <v>76</v>
       </c>
       <c r="C18" s="12">
-        <v>327196</v>
+        <v>327980</v>
       </c>
       <c r="D18" s="12">
-        <v>2816</v>
+        <v>2956</v>
       </c>
       <c r="E18" s="16">
-        <f t="shared" si="0"/>
-        <v>0.86064621816892628</v>
+        <v>0.90127446795536315</v>
       </c>
       <c r="F18" s="11">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -1924,17 +1920,16 @@
         <v>77</v>
       </c>
       <c r="C19" s="12">
-        <v>381933</v>
+        <v>384834</v>
       </c>
       <c r="D19" s="12">
-        <v>5252</v>
+        <v>5588</v>
       </c>
       <c r="E19" s="16">
-        <f t="shared" si="0"/>
-        <v>1.3751102942139066</v>
+        <v>1.452054652135726</v>
       </c>
       <c r="F19" s="11">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1942,17 +1937,16 @@
         <v>78</v>
       </c>
       <c r="C20" s="12">
-        <v>464626</v>
+        <v>472823</v>
       </c>
       <c r="D20" s="12">
-        <v>3682</v>
+        <v>3919</v>
       </c>
       <c r="E20" s="16">
-        <f t="shared" si="0"/>
-        <v>0.79246533771248284</v>
+        <v>0.82885138836308725</v>
       </c>
       <c r="F20" s="11">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -1960,17 +1954,16 @@
         <v>79</v>
       </c>
       <c r="C21" s="12">
-        <v>506459</v>
+        <v>512969</v>
       </c>
       <c r="D21" s="12">
-        <v>3092</v>
+        <v>3204</v>
       </c>
       <c r="E21" s="16">
-        <f t="shared" si="0"/>
-        <v>0.61051338805312971</v>
+        <v>0.62459914731689448</v>
       </c>
       <c r="F21" s="11">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1978,17 +1971,16 @@
         <v>80</v>
       </c>
       <c r="C22" s="12">
-        <v>510551</v>
+        <v>513572</v>
       </c>
       <c r="D22" s="12">
-        <v>2992</v>
+        <v>3042</v>
       </c>
       <c r="E22" s="16">
-        <f t="shared" si="0"/>
-        <v>0.58603352064730063</v>
+        <v>0.59232201132460494</v>
       </c>
       <c r="F22" s="11">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -1996,17 +1988,16 @@
         <v>81</v>
       </c>
       <c r="C23" s="12">
-        <v>538701</v>
+        <v>544219</v>
       </c>
       <c r="D23" s="12">
-        <v>3497</v>
+        <v>3608</v>
       </c>
       <c r="E23" s="16">
-        <f t="shared" si="0"/>
-        <v>0.64915416901026735</v>
+        <v>0.66296840058873363</v>
       </c>
       <c r="F23" s="11">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -2014,17 +2005,16 @@
         <v>82</v>
       </c>
       <c r="C24" s="12">
-        <v>553742</v>
+        <v>556634</v>
       </c>
       <c r="D24" s="12">
-        <v>4458</v>
+        <v>4537</v>
       </c>
       <c r="E24" s="16">
-        <f t="shared" si="0"/>
-        <v>0.80506806418873778</v>
+        <v>0.81507777103087486</v>
       </c>
       <c r="F24" s="11">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -2032,17 +2022,16 @@
         <v>83</v>
       </c>
       <c r="C25" s="12">
-        <v>586967</v>
+        <v>589201</v>
       </c>
       <c r="D25" s="12">
-        <v>5738</v>
+        <v>5888</v>
       </c>
       <c r="E25" s="16">
-        <f t="shared" si="0"/>
-        <v>0.9775677337908264</v>
+        <v>0.99931941731259788</v>
       </c>
       <c r="F25" s="11">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -2050,17 +2039,16 @@
         <v>84</v>
       </c>
       <c r="C26" s="12">
-        <v>717123</v>
+        <v>719476</v>
       </c>
       <c r="D26" s="12">
-        <v>7263</v>
+        <v>7374</v>
       </c>
       <c r="E26" s="16">
-        <f t="shared" si="0"/>
-        <v>1.0127969678841706</v>
+        <v>1.0249125752631083</v>
       </c>
       <c r="F26" s="11">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -2068,17 +2056,16 @@
         <v>85</v>
       </c>
       <c r="C27" s="12">
-        <v>835384</v>
+        <v>871191</v>
       </c>
       <c r="D27" s="12">
-        <v>8121</v>
+        <v>8545</v>
       </c>
       <c r="E27" s="16">
-        <f t="shared" si="0"/>
-        <v>0.97212778793943855</v>
+        <v>0.98084117030593754</v>
       </c>
       <c r="F27" s="11">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -2086,17 +2073,16 @@
         <v>86</v>
       </c>
       <c r="C28" s="12">
-        <v>1029715</v>
+        <v>1034449</v>
       </c>
       <c r="D28" s="12">
-        <v>8766</v>
+        <v>8868</v>
       </c>
       <c r="E28" s="16">
-        <f t="shared" si="0"/>
-        <v>0.85130351602142351</v>
+        <v>0.85726797551160094</v>
       </c>
       <c r="F28" s="11">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -2104,17 +2090,16 @@
         <v>87</v>
       </c>
       <c r="C29" s="12">
-        <v>1091207</v>
+        <v>1133623</v>
       </c>
       <c r="D29" s="12">
-        <v>8061</v>
+        <v>8273</v>
       </c>
       <c r="E29" s="16">
-        <f t="shared" si="0"/>
-        <v>0.73872326698784008</v>
+        <v>0.72978406401422702</v>
       </c>
       <c r="F29" s="11">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -2122,17 +2107,16 @@
         <v>88</v>
       </c>
       <c r="C30" s="12">
-        <v>1043713</v>
+        <v>1052942</v>
       </c>
       <c r="D30" s="12">
-        <v>8072</v>
+        <v>8203</v>
       </c>
       <c r="E30" s="16">
-        <f t="shared" si="0"/>
-        <v>0.77339268553711604</v>
+        <v>0.77905525660482722</v>
       </c>
       <c r="F30" s="11">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -2140,17 +2124,16 @@
         <v>89</v>
       </c>
       <c r="C31" s="12">
-        <v>1133737</v>
+        <v>1148465</v>
       </c>
       <c r="D31" s="12">
-        <v>9855</v>
+        <v>10403</v>
       </c>
       <c r="E31" s="16">
-        <f t="shared" si="0"/>
-        <v>0.86924921741109262</v>
+        <v>0.90581776545214709</v>
       </c>
       <c r="F31" s="11">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -2158,17 +2141,16 @@
         <v>90</v>
       </c>
       <c r="C32" s="12">
-        <v>1090740</v>
+        <v>1147879</v>
       </c>
       <c r="D32" s="12">
-        <v>12937</v>
+        <v>13647</v>
       </c>
       <c r="E32" s="16">
-        <f t="shared" si="0"/>
-        <v>1.1860755083704642</v>
+        <v>1.1888883758654005</v>
       </c>
       <c r="F32" s="11">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -2176,17 +2158,16 @@
         <v>91</v>
       </c>
       <c r="C33" s="12">
-        <v>1154700</v>
+        <v>1220279</v>
       </c>
       <c r="D33" s="12">
-        <v>14140</v>
+        <v>15178</v>
       </c>
       <c r="E33" s="16">
-        <f t="shared" si="0"/>
-        <v>1.2245604919026587</v>
+        <v>1.2438139146867233</v>
       </c>
       <c r="F33" s="11">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -2194,17 +2175,16 @@
         <v>92</v>
       </c>
       <c r="C34" s="12">
-        <v>1112967</v>
+        <v>1129127</v>
       </c>
       <c r="D34" s="12">
-        <v>19407</v>
+        <v>19930</v>
       </c>
       <c r="E34" s="16">
-        <f t="shared" si="0"/>
-        <v>1.7437174687120103</v>
+        <v>1.7650804559628812</v>
       </c>
       <c r="F34" s="11">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -2212,17 +2192,16 @@
         <v>93</v>
       </c>
       <c r="C35" s="12">
-        <v>1188338</v>
+        <v>1218988</v>
       </c>
       <c r="D35" s="12">
-        <v>29567</v>
+        <v>30220</v>
       </c>
       <c r="E35" s="16">
-        <f t="shared" si="0"/>
-        <v>2.4880968209381504</v>
+        <v>2.4791056187591676</v>
       </c>
       <c r="F35" s="11">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -2230,17 +2209,16 @@
         <v>94</v>
       </c>
       <c r="C36" s="12">
-        <v>1220909</v>
+        <v>1284349</v>
       </c>
       <c r="D36" s="12">
-        <v>44046</v>
+        <v>46000</v>
       </c>
       <c r="E36" s="16">
-        <f t="shared" si="0"/>
-        <v>3.6076398814326045</v>
+        <v>3.581581018866367</v>
       </c>
       <c r="F36" s="11">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -2248,17 +2226,16 @@
         <v>95</v>
       </c>
       <c r="C37" s="12">
-        <v>1373753</v>
+        <v>1445463</v>
       </c>
       <c r="D37" s="12">
-        <v>77006</v>
+        <v>80097</v>
       </c>
       <c r="E37" s="16">
-        <f t="shared" si="0"/>
-        <v>5.605520060738721</v>
+        <v>5.5412694755936336</v>
       </c>
       <c r="F37" s="11">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -2266,17 +2243,16 @@
         <v>96</v>
       </c>
       <c r="C38" s="12">
-        <v>1593278</v>
+        <v>1663992</v>
       </c>
       <c r="D38" s="12">
-        <v>115235</v>
+        <v>118111</v>
       </c>
       <c r="E38" s="16">
-        <f t="shared" si="0"/>
-        <v>7.2325733487815675</v>
+        <v>7.0980509521680393</v>
       </c>
       <c r="F38" s="11">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -2284,17 +2260,16 @@
         <v>97</v>
       </c>
       <c r="C39" s="12">
-        <v>1598527</v>
+        <v>1634729</v>
       </c>
       <c r="D39" s="12">
-        <v>124869</v>
+        <v>128537</v>
       </c>
       <c r="E39" s="16">
-        <f t="shared" si="0"/>
-        <v>7.8115039658385497</v>
+        <v>7.8628934826506418</v>
       </c>
       <c r="F39" s="11">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -2302,17 +2277,16 @@
         <v>98</v>
       </c>
       <c r="C40" s="12">
-        <v>1396088</v>
+        <v>1467454</v>
       </c>
       <c r="D40" s="12">
-        <v>125200</v>
+        <v>128986</v>
       </c>
       <c r="E40" s="16">
-        <f t="shared" si="0"/>
-        <v>8.967916062597773</v>
+        <v>8.789781485484383</v>
       </c>
       <c r="F40" s="11">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -2320,17 +2294,16 @@
         <v>99</v>
       </c>
       <c r="C41" s="12">
-        <v>1367570</v>
+        <v>1400145</v>
       </c>
       <c r="D41" s="12">
-        <v>127742</v>
+        <v>131185</v>
       </c>
       <c r="E41" s="16">
-        <f t="shared" si="0"/>
-        <v>9.3408015677442471</v>
+        <v>9.3693867420874266</v>
       </c>
       <c r="F41" s="11">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -2338,17 +2311,16 @@
         <v>100</v>
       </c>
       <c r="C42" s="12">
-        <v>1353980</v>
+        <v>1381117</v>
       </c>
       <c r="D42" s="12">
-        <v>125451</v>
+        <v>128882</v>
       </c>
       <c r="E42" s="16">
-        <f t="shared" si="0"/>
-        <v>9.2653510391586291</v>
+        <v>9.3317220771303226</v>
       </c>
       <c r="F42" s="11">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -2356,17 +2328,16 @@
         <v>101</v>
       </c>
       <c r="C43" s="12">
-        <v>1329716</v>
+        <v>1395790</v>
       </c>
       <c r="D43" s="12">
-        <v>135062</v>
+        <v>138305</v>
       </c>
       <c r="E43" s="16">
-        <f t="shared" si="0"/>
-        <v>10.157206501237859</v>
+        <v>9.9087255246133008</v>
       </c>
       <c r="F43" s="11">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
@@ -2374,17 +2345,16 @@
         <v>102</v>
       </c>
       <c r="C44" s="12">
-        <v>1445671</v>
+        <v>1516038</v>
       </c>
       <c r="D44" s="12">
-        <v>165953</v>
+        <v>169520</v>
       </c>
       <c r="E44" s="16">
-        <f t="shared" si="0"/>
-        <v>11.479306149186087</v>
+        <v>11.181777765464981</v>
       </c>
       <c r="F44" s="11">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
@@ -2392,17 +2362,16 @@
         <v>103</v>
       </c>
       <c r="C45" s="12">
-        <v>1613358</v>
+        <v>1672033</v>
       </c>
       <c r="D45" s="12">
-        <v>185724</v>
+        <v>188283</v>
       </c>
       <c r="E45" s="16">
-        <f t="shared" si="0"/>
-        <v>11.511642177371668</v>
+        <v>11.260722724970142</v>
       </c>
       <c r="F45" s="11">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -2410,17 +2379,16 @@
         <v>104</v>
       </c>
       <c r="C46" s="12">
-        <v>1077066</v>
+        <v>1091427</v>
       </c>
       <c r="D46" s="12">
-        <v>138761</v>
+        <v>141427</v>
       </c>
       <c r="E46" s="16">
-        <f t="shared" si="0"/>
-        <v>12.883240209977847</v>
+        <v>12.957989860980165</v>
       </c>
       <c r="F46" s="11">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -2428,17 +2396,16 @@
         <v>105</v>
       </c>
       <c r="C47" s="12">
-        <v>806908</v>
+        <v>844502</v>
       </c>
       <c r="D47" s="12">
-        <v>128349</v>
+        <v>129872</v>
       </c>
       <c r="E47" s="16">
-        <f t="shared" si="0"/>
-        <v>15.906274321236127</v>
+        <v>15.378530779086372</v>
       </c>
       <c r="F47" s="11">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
@@ -2446,17 +2413,16 @@
         <v>106</v>
       </c>
       <c r="C48" s="12">
-        <v>1214379</v>
+        <v>1227527</v>
       </c>
       <c r="D48" s="12">
-        <v>154988</v>
+        <v>157569</v>
       </c>
       <c r="E48" s="16">
-        <f t="shared" si="0"/>
-        <v>12.762737168544581</v>
+        <v>12.8362960651782</v>
       </c>
       <c r="F48" s="11">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
@@ -2464,17 +2430,16 @@
         <v>108</v>
       </c>
       <c r="C49" s="12">
-        <v>1162475</v>
+        <v>1184400</v>
       </c>
       <c r="D49" s="12">
-        <v>121341</v>
+        <v>123851</v>
       </c>
       <c r="E49" s="16">
-        <f t="shared" si="0"/>
-        <v>10.438159960429257</v>
+        <v>10.456855791962175</v>
       </c>
       <c r="F49" s="11">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
@@ -2482,47 +2447,63 @@
         <v>110</v>
       </c>
       <c r="C50" s="12">
-        <v>1068323</v>
+        <v>1100346</v>
       </c>
       <c r="D50" s="12">
-        <v>106488</v>
+        <v>109391</v>
       </c>
       <c r="E50" s="16">
-        <f t="shared" si="0"/>
-        <v>9.9677719191667702</v>
+        <v>9.9415093070725025</v>
       </c>
       <c r="F50" s="11">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="12">
+        <v>1116314</v>
+      </c>
+      <c r="D51" s="12">
+        <v>95187</v>
+      </c>
+      <c r="E51" s="16">
+        <v>8.5269019290271384</v>
+      </c>
+      <c r="F51" s="11">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="14">
-        <f>SUM(C4:C50)</f>
-        <v>38533736</v>
-      </c>
-      <c r="D51" s="14">
-        <f>SUM(D4:D50)</f>
-        <v>2249854</v>
-      </c>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="31" t="s">
+      <c r="C52" s="14">
+        <f>SUM(C4:C51)</f>
+        <v>40705522</v>
+      </c>
+      <c r="D52" s="14">
+        <f>SUM(D4:D51)</f>
+        <v>2398614</v>
+      </c>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="B53:F53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2531,10 +2512,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:E49"/>
+  <dimension ref="A2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3362,6 +3343,23 @@
         <v>2207810</v>
       </c>
     </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="23">
+        <v>173</v>
+      </c>
+      <c r="C50" s="27">
+        <v>346155</v>
+      </c>
+      <c r="D50" s="27">
+        <v>2329447</v>
+      </c>
+      <c r="E50" s="27">
+        <v>2237756</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3370,10 +3368,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3880,6 +3878,17 @@
         <v>11980</v>
       </c>
     </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="22">
+        <v>42</v>
+      </c>
+      <c r="B44" s="22">
+        <v>4</v>
+      </c>
+      <c r="C44" s="27">
+        <v>5572</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add RKI data downloaded 2021-03-21--19-15-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Testzahlen-gesamt.xlsx
+++ b/rki-data/RKI-Testzahlen-gesamt.xlsx
@@ -2,10 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D7A13C-4984-452F-80C5-4278618EAD05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\4.6.Laborergebnisse\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CA0E44-26E0-45CC-A6B9-5444A3DE4E6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="25950" windowHeight="5385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="22650" windowHeight="10185" tabRatio="319" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_Erläuterungen" sheetId="7" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="73">
   <si>
     <t>Das RKI erfasst wöchentlich die SARS-CoV-2-Testzahlen. Hierfür werden deutschlandweit Daten von Universitätskliniken, Forschungseinrichtungen sowie klinischen und ambulanten Laboren zusammengeführt. Die Erfassung basiert auf einer freiwilligen Mitteilung der Labore und erfolgt über eine webbasierte Plattform (VOXCO, RKI-Testlaborabfrage) oder in Zusammenarbeit mit der am RKI etablierten, laborbasierten SARS-CoV-2-Surveillance (eine Erweiterung der Antibiotika-Resistenz-Surveillance, ARS), dem Netzwerk für respiratorische Viren (RespVir) sowie der Abfrage eines labormedizinischen Berufsverbands. Die Erfassung liefert Hinweise zur aktuellen Situation in den Laboren, erlaubt aber keine detaillierten Auswertungen oder Vergleiche mit den gemeldeten Fallzahlen.</t>
   </si>
@@ -148,130 +153,82 @@
     <t>45/2020</t>
   </si>
   <si>
-    <t>46/2020*</t>
-  </si>
-  <si>
-    <t>47/2020*</t>
-  </si>
-  <si>
-    <t>48/2020*</t>
-  </si>
-  <si>
-    <t>49/2020*</t>
-  </si>
-  <si>
-    <t>50/2020*</t>
-  </si>
-  <si>
-    <t>51/2020*</t>
-  </si>
-  <si>
-    <t>52/2020*</t>
-  </si>
-  <si>
-    <t>53/2020*</t>
-  </si>
-  <si>
-    <t>1/2021*</t>
-  </si>
-  <si>
-    <t>2/2021*</t>
-  </si>
-  <si>
-    <t>3/2021*</t>
-  </si>
-  <si>
-    <t>4/2021*</t>
-  </si>
-  <si>
-    <t>5/2021*</t>
-  </si>
-  <si>
-    <t>6/2021*</t>
-  </si>
-  <si>
-    <t>7/2021*</t>
-  </si>
-  <si>
-    <t>8/2021*</t>
-  </si>
-  <si>
-    <t>9/2021*</t>
-  </si>
-  <si>
     <t>Summe</t>
   </si>
   <si>
-    <t>Bis einschließlich KW52/2020</t>
+    <t>Bis einschließlich KW53/2020</t>
+  </si>
+  <si>
+    <t>1/2021</t>
+  </si>
+  <si>
+    <t>2/2021</t>
+  </si>
+  <si>
+    <t>3/2021</t>
+  </si>
+  <si>
+    <t>4/2021</t>
+  </si>
+  <si>
+    <t>5/2021</t>
+  </si>
+  <si>
+    <t>6/2021</t>
+  </si>
+  <si>
+    <t>7/2021</t>
+  </si>
+  <si>
+    <t>8/2021</t>
+  </si>
+  <si>
+    <t>9/2021</t>
+  </si>
+  <si>
+    <t>10/2021</t>
+  </si>
+  <si>
+    <t>KW, für die die Angabe prognostisch erfolgt ist</t>
+  </si>
+  <si>
+    <t>Anzahl übermittelnde Labore</t>
+  </si>
+  <si>
+    <t>Testkapazität pro Tag</t>
+  </si>
+  <si>
+    <t>Theoretische wöchentliche Kapazität anhand von Wochenarbeitstagen</t>
+  </si>
+  <si>
+    <t>Reale Testkapazität zum Zeitpunkt der Abfrage</t>
+  </si>
+  <si>
+    <t>46/2020</t>
+  </si>
+  <si>
+    <t>47/2020</t>
+  </si>
+  <si>
+    <t>48/2020</t>
+  </si>
+  <si>
+    <t>49/2020</t>
+  </si>
+  <si>
+    <t>50/2020</t>
+  </si>
+  <si>
+    <t>51/2020</t>
+  </si>
+  <si>
+    <t>52/2020</t>
   </si>
   <si>
     <t>53/2020</t>
   </si>
   <si>
-    <t>1/2021</t>
-  </si>
-  <si>
-    <t>2/2021</t>
-  </si>
-  <si>
-    <t>3/2021</t>
-  </si>
-  <si>
-    <t>4/2021</t>
-  </si>
-  <si>
-    <t>5/2021</t>
-  </si>
-  <si>
-    <t>6/2021</t>
-  </si>
-  <si>
-    <t>7/2021</t>
-  </si>
-  <si>
-    <t>8/2021</t>
-  </si>
-  <si>
-    <t>9/2021</t>
-  </si>
-  <si>
-    <t>KW, für die die Angabe prognostisch erfolgt ist</t>
-  </si>
-  <si>
-    <t>Anzahl übermittelnde Labore</t>
-  </si>
-  <si>
-    <t>Testkapazität pro Tag</t>
-  </si>
-  <si>
-    <t>Theoretische wöchentliche Kapazität anhand von Wochenarbeitstagen</t>
-  </si>
-  <si>
-    <t>Reale Testkapazität zum Zeitpunkt der Abfrage</t>
-  </si>
-  <si>
-    <t>46/2020</t>
-  </si>
-  <si>
-    <t>47/2020</t>
-  </si>
-  <si>
-    <t>48/2020</t>
-  </si>
-  <si>
-    <t>49/2020</t>
-  </si>
-  <si>
-    <t>50/2020</t>
-  </si>
-  <si>
-    <t>51/2020</t>
-  </si>
-  <si>
-    <t>52/2020</t>
-  </si>
-  <si>
-    <t>10/2021</t>
+    <t>11/2021</t>
   </si>
   <si>
     <t>Labore mit Rückstau</t>
@@ -287,16 +244,17 @@
   </si>
   <si>
     <t xml:space="preserve">Zusätzlich zur Anzahl durchgeführter Tests werden in der RKI-Testlaborabfrage und durch einen labormedizinischen Berufsverband Angaben zur täglichen (aktuellen) Testkapazität, zur Reichweite sowie zu möglichen Probenrückstaus befragt. Die Reichweite gibt an, wie viele Arbeitstage ein Labor unter Vollauslastung  der angegebenen maximalen Testkapazität unter Berücksichtigung aller notwendigen Ressourcen (Entnahmematerial, Testreagenzien, Personal u. a.) zum Zeitpunkt der Abfrage arbeiten kann. Da die Reichweite stark  vom Vorhandensein von Testreagenzien abhängig ist, stellt die Angabe eine Momentaufnahme in einem dynamischen System dar (s. Testkapazitäten, Probenrückstau). </t>
-  </si>
-  <si>
-    <t>*Ab 03. November 2020 geänderte Testkriterien, Daten nicht direkt mit Vorwochen vergleichbar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.00_ ;\-0.00\ "/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -307,6 +265,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -334,7 +299,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -342,34 +307,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -390,11 +347,26 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -403,17 +375,18 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{AC792CF2-4318-4D97-827E-F26285CDD0CB}"/>
+    <cellStyle name="Standard 2" xfId="2" xr:uid="{3EFF19E7-C5B7-44E9-A0B9-6F4F2BE4905E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -432,23 +405,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>175895</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>59055</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>261257</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Grafik 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7435B976-D364-4291-9EE0-F4207882B5FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60443AA9-CE07-4914-99AC-138FC2548922}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -470,8 +443,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4248150" y="890270"/>
-          <a:ext cx="9067800" cy="4836160"/>
+          <a:off x="4803321" y="1524000"/>
+          <a:ext cx="10058400" cy="4470400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -779,14 +752,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75916A43-D511-44B5-BA57-BE474A7C5110}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABAE72F-11AC-453B-BAF1-7F0DE6F6E080}">
   <dimension ref="A3:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="140.85546875" style="5" customWidth="1"/>
     <col min="2" max="16384" width="11.42578125" style="3"/>
@@ -799,12 +772,12 @@
     </row>
     <row r="4" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -815,22 +788,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:E57"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -846,11 +819,8 @@
       <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -862,11 +832,8 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -882,11 +849,8 @@
       <c r="E3" s="7">
         <v>118</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -902,11 +866,8 @@
       <c r="E4" s="7">
         <v>154</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -922,11 +883,8 @@
       <c r="E5" s="7">
         <v>159</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -942,11 +900,8 @@
       <c r="E6" s="7">
         <v>163</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -962,11 +917,8 @@
       <c r="E7" s="7">
         <v>175</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -982,11 +934,8 @@
       <c r="E8" s="7">
         <v>172</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -1002,11 +951,8 @@
       <c r="E9" s="7">
         <v>180</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
@@ -1022,11 +968,8 @@
       <c r="E10" s="7">
         <v>178</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1042,11 +985,8 @@
       <c r="E11" s="7">
         <v>181</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -1062,11 +1002,8 @@
       <c r="E12" s="7">
         <v>183</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1082,11 +1019,8 @@
       <c r="E13" s="7">
         <v>181</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
@@ -1102,11 +1036,8 @@
       <c r="E14" s="7">
         <v>175</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1122,11 +1053,8 @@
       <c r="E15" s="7">
         <v>178</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -1142,11 +1070,8 @@
       <c r="E16" s="7">
         <v>175</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
@@ -1162,11 +1087,8 @@
       <c r="E17" s="7">
         <v>175</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
@@ -1182,11 +1104,8 @@
       <c r="E18" s="7">
         <v>182</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>23</v>
       </c>
@@ -1202,11 +1121,8 @@
       <c r="E19" s="7">
         <v>154</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -1222,11 +1138,8 @@
       <c r="E20" s="7">
         <v>182</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
@@ -1242,11 +1155,8 @@
       <c r="E21" s="7">
         <v>182</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
@@ -1262,11 +1172,8 @@
       <c r="E22" s="7">
         <v>187</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
@@ -1282,11 +1189,8 @@
       <c r="E23" s="7">
         <v>175</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
@@ -1302,11 +1206,8 @@
       <c r="E24" s="7">
         <v>174</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
@@ -1322,11 +1223,8 @@
       <c r="E25" s="7">
         <v>189</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
@@ -1342,11 +1240,8 @@
       <c r="E26" s="7">
         <v>197</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
@@ -1362,11 +1257,8 @@
       <c r="E27" s="7">
         <v>196</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>32</v>
       </c>
@@ -1382,11 +1274,8 @@
       <c r="E28" s="7">
         <v>195</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>33</v>
       </c>
@@ -1402,11 +1291,8 @@
       <c r="E29" s="7">
         <v>197</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
@@ -1422,11 +1308,8 @@
       <c r="E30" s="7">
         <v>206</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>35</v>
       </c>
@@ -1442,11 +1325,8 @@
       <c r="E31" s="7">
         <v>200</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>36</v>
       </c>
@@ -1462,11 +1342,8 @@
       <c r="E32" s="7">
         <v>198</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>37</v>
       </c>
@@ -1482,11 +1359,8 @@
       <c r="E33" s="7">
         <v>198</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>38</v>
       </c>
@@ -1502,11 +1376,8 @@
       <c r="E34" s="7">
         <v>205</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>39</v>
       </c>
@@ -1522,11 +1393,8 @@
       <c r="E35" s="7">
         <v>209</v>
       </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>40</v>
       </c>
@@ -1542,11 +1410,8 @@
       <c r="E36" s="7">
         <v>210</v>
       </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>41</v>
       </c>
@@ -1562,13 +1427,10 @@
       <c r="E37" s="7">
         <v>208</v>
       </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B38" s="8">
         <v>1467454</v>
@@ -1582,13 +1444,10 @@
       <c r="E38" s="7">
         <v>206</v>
       </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B39" s="8">
         <v>1400145</v>
@@ -1602,13 +1461,10 @@
       <c r="E39" s="7">
         <v>204</v>
       </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B40" s="8">
         <v>1381117</v>
@@ -1622,13 +1478,10 @@
       <c r="E40" s="7">
         <v>206</v>
       </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B41" s="8">
         <v>1395790</v>
@@ -1642,13 +1495,10 @@
       <c r="E41" s="7">
         <v>208</v>
       </c>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B42" s="8">
         <v>1516038</v>
@@ -1662,13 +1512,10 @@
       <c r="E42" s="7">
         <v>206</v>
       </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B43" s="8">
         <v>1672033</v>
@@ -1682,13 +1529,10 @@
       <c r="E43" s="7">
         <v>212</v>
       </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B44" s="8">
         <v>1090372</v>
@@ -1702,13 +1546,10 @@
       <c r="E44" s="7">
         <v>208</v>
       </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B45" s="8">
         <v>845729</v>
@@ -1722,13 +1563,10 @@
       <c r="E45" s="7">
         <v>205</v>
       </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>50</v>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="B46" s="8">
         <v>1231405</v>
@@ -1742,13 +1580,10 @@
       <c r="E46" s="7">
         <v>206</v>
       </c>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>51</v>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="B47" s="8">
         <v>1187564</v>
@@ -1762,13 +1597,10 @@
       <c r="E47" s="7">
         <v>206</v>
       </c>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>52</v>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>46</v>
       </c>
       <c r="B48" s="8">
         <v>1110190</v>
@@ -1782,13 +1614,10 @@
       <c r="E48" s="7">
         <v>207</v>
       </c>
-      <c r="F48" s="7"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>53</v>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>47</v>
       </c>
       <c r="B49" s="8">
         <v>1148018</v>
@@ -1802,13 +1631,10 @@
       <c r="E49" s="7">
         <v>207</v>
       </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>54</v>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="B50" s="8">
         <v>1097419</v>
@@ -1822,13 +1648,10 @@
       <c r="E50" s="7">
         <v>207</v>
       </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>55</v>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="B51" s="8">
         <v>1056768</v>
@@ -1842,13 +1665,10 @@
       <c r="E51" s="7">
         <v>211</v>
       </c>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>56</v>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="B52" s="11">
         <v>1098665</v>
@@ -1862,13 +1682,10 @@
       <c r="E52" s="10">
         <v>205</v>
       </c>
-      <c r="F52" s="10"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>57</v>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="B53" s="11">
         <v>1170335</v>
@@ -1882,324 +1699,60 @@
       <c r="E53" s="7">
         <v>209</v>
       </c>
-      <c r="F53" s="10"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-    </row>
-    <row r="54" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
-        <v>58</v>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="B54" s="11">
-        <v>1136825</v>
+        <v>1147877</v>
       </c>
       <c r="C54" s="11">
-        <v>70991</v>
+        <v>71377</v>
       </c>
       <c r="D54" s="12">
-        <v>6.2446726628988634</v>
+        <v>6.2181749438310892</v>
       </c>
       <c r="E54" s="10">
-        <v>201</v>
-      </c>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" s="13">
-        <v>46319641</v>
-      </c>
-      <c r="C55" s="13">
-        <v>2762316</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A57:E57"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="8">
-        <v>35236723</v>
-      </c>
-      <c r="C2" s="8">
-        <v>1783035</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="8">
-        <v>845729</v>
-      </c>
-      <c r="C3" s="8">
-        <v>129930</v>
-      </c>
-      <c r="D3" s="16">
-        <v>15.363077297810529</v>
-      </c>
-      <c r="E3" s="17">
-        <v>205</v>
-      </c>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="8">
-        <v>1231405</v>
-      </c>
-      <c r="C4" s="8">
-        <v>157772</v>
-      </c>
-      <c r="D4" s="16">
-        <v>12.812356617035011</v>
-      </c>
-      <c r="E4" s="17">
-        <v>206</v>
-      </c>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1187564</v>
-      </c>
-      <c r="C5" s="8">
-        <v>124037</v>
-      </c>
-      <c r="D5" s="16">
-        <v>10.44465814052969</v>
-      </c>
-      <c r="E5" s="17">
-        <v>206</v>
-      </c>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1110190</v>
-      </c>
-      <c r="C6" s="8">
-        <v>110014</v>
-      </c>
-      <c r="D6" s="16">
-        <v>9.9094749547374779</v>
-      </c>
-      <c r="E6" s="17">
-        <v>207</v>
-      </c>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1148018</v>
-      </c>
-      <c r="C7" s="8">
-        <v>97256</v>
-      </c>
-      <c r="D7" s="16">
-        <v>8.4716441728265597</v>
-      </c>
-      <c r="E7" s="17">
-        <v>207</v>
-      </c>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1097419</v>
-      </c>
-      <c r="C8" s="8">
-        <v>82288</v>
-      </c>
-      <c r="D8" s="16">
-        <v>7.4983210605976387</v>
-      </c>
-      <c r="E8" s="17">
-        <v>207</v>
-      </c>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="8">
-        <v>1056768</v>
-      </c>
-      <c r="C9" s="8">
-        <v>67774</v>
-      </c>
-      <c r="D9" s="16">
-        <v>6.4133281855620154</v>
-      </c>
-      <c r="E9" s="17">
-        <v>211</v>
-      </c>
-      <c r="F9" s="17"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1098665</v>
-      </c>
-      <c r="C10" s="8">
-        <v>67211</v>
-      </c>
-      <c r="D10" s="16">
-        <v>6.1175153481725548</v>
-      </c>
-      <c r="E10" s="17">
-        <v>205</v>
-      </c>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1170335</v>
-      </c>
-      <c r="C11" s="8">
-        <v>72008</v>
-      </c>
-      <c r="D11" s="16">
-        <v>6.1527682244827337</v>
-      </c>
-      <c r="E11" s="17">
-        <v>209</v>
-      </c>
-      <c r="F11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="8">
-        <v>1136825</v>
-      </c>
-      <c r="C12" s="8">
-        <v>70991</v>
-      </c>
-      <c r="D12" s="16">
-        <v>6.2446726628988634</v>
-      </c>
-      <c r="E12" s="17">
-        <v>201</v>
-      </c>
-      <c r="F12" s="17"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="13">
-        <v>46319641</v>
-      </c>
-      <c r="C13" s="13">
-        <v>2762316</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="11">
+        <v>1248100</v>
+      </c>
+      <c r="C55" s="11">
+        <v>84480</v>
+      </c>
+      <c r="D55" s="15">
+        <v>6.7686884063776942</v>
+      </c>
+      <c r="E55" s="10">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" s="13">
+        <v>47578793</v>
+      </c>
+      <c r="C56" s="13">
+        <v>2847182</v>
+      </c>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2207,41 +1760,276 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F56"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="5" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="8">
+        <v>36082452</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1912965</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1231405</v>
+      </c>
+      <c r="C3" s="8">
+        <v>157772</v>
+      </c>
+      <c r="D3" s="21">
+        <v>12.812356617035011</v>
+      </c>
+      <c r="E3" s="22">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1187564</v>
+      </c>
+      <c r="C4" s="8">
+        <v>124037</v>
+      </c>
+      <c r="D4" s="21">
+        <v>10.44465814052969</v>
+      </c>
+      <c r="E4" s="22">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1110190</v>
+      </c>
+      <c r="C5" s="8">
+        <v>110014</v>
+      </c>
+      <c r="D5" s="21">
+        <v>9.9094749547374779</v>
+      </c>
+      <c r="E5" s="22">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1148018</v>
+      </c>
+      <c r="C6" s="8">
+        <v>97256</v>
+      </c>
+      <c r="D6" s="21">
+        <v>8.4716441728265597</v>
+      </c>
+      <c r="E6" s="22">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1097419</v>
+      </c>
+      <c r="C7" s="8">
+        <v>82288</v>
+      </c>
+      <c r="D7" s="21">
+        <v>7.4983210605976387</v>
+      </c>
+      <c r="E7" s="22">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1056768</v>
+      </c>
+      <c r="C8" s="8">
+        <v>67774</v>
+      </c>
+      <c r="D8" s="21">
+        <v>6.4133281855620154</v>
+      </c>
+      <c r="E8" s="22">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1098665</v>
+      </c>
+      <c r="C9" s="8">
+        <v>67211</v>
+      </c>
+      <c r="D9" s="21">
+        <v>6.1175153481725548</v>
+      </c>
+      <c r="E9" s="22">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1170335</v>
+      </c>
+      <c r="C10" s="8">
+        <v>72008</v>
+      </c>
+      <c r="D10" s="21">
+        <v>6.1527682244827337</v>
+      </c>
+      <c r="E10" s="22">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1147877</v>
+      </c>
+      <c r="C11" s="8">
+        <v>71377</v>
+      </c>
+      <c r="D11" s="21">
+        <v>6.2181749438310892</v>
+      </c>
+      <c r="E11" s="22">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1248100</v>
+      </c>
+      <c r="C12" s="8">
+        <v>84480</v>
+      </c>
+      <c r="D12" s="21">
+        <v>6.7686884063776942</v>
+      </c>
+      <c r="E12" s="22">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="13">
+        <v>47578793</v>
+      </c>
+      <c r="C13" s="13">
+        <v>2847182</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:E57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55:E55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -2257,9 +2045,8 @@
       <c r="E2" s="8">
         <v>40950</v>
       </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2275,9 +2062,8 @@
       <c r="E3" s="8">
         <v>119700</v>
       </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -2293,9 +2079,8 @@
       <c r="E4" s="8">
         <v>367630</v>
       </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2311,9 +2096,8 @@
       <c r="E5" s="8">
         <v>531380</v>
       </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
@@ -2329,9 +2113,8 @@
       <c r="E6" s="8">
         <v>664960</v>
       </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -2347,9 +2130,8 @@
       <c r="E7" s="8">
         <v>670650</v>
       </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -2365,9 +2147,8 @@
       <c r="E8" s="8">
         <v>700399</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
@@ -2383,9 +2164,8 @@
       <c r="E9" s="8">
         <v>730541</v>
       </c>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
@@ -2401,9 +2181,8 @@
       <c r="E10" s="8">
         <v>831816</v>
       </c>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
@@ -2419,9 +2198,8 @@
       <c r="E11" s="8">
         <v>873162</v>
       </c>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -2437,9 +2215,8 @@
       <c r="E12" s="8">
         <v>882561</v>
       </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
@@ -2455,9 +2232,8 @@
       <c r="E13" s="8">
         <v>880441</v>
       </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>19</v>
       </c>
@@ -2473,9 +2249,8 @@
       <c r="E14" s="8">
         <v>939801</v>
       </c>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
@@ -2491,9 +2266,8 @@
       <c r="E15" s="8">
         <v>974698</v>
       </c>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>21</v>
       </c>
@@ -2509,9 +2283,8 @@
       <c r="E16" s="8">
         <v>996309</v>
       </c>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
@@ -2527,9 +2300,8 @@
       <c r="E17" s="8">
         <v>994060</v>
       </c>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>23</v>
       </c>
@@ -2545,9 +2317,8 @@
       <c r="E18" s="8">
         <v>1003758</v>
       </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>24</v>
       </c>
@@ -2563,9 +2334,8 @@
       <c r="E19" s="8">
         <v>1020962</v>
       </c>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>25</v>
       </c>
@@ -2581,9 +2351,8 @@
       <c r="E20" s="8">
         <v>1041871</v>
       </c>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>26</v>
       </c>
@@ -2599,9 +2368,8 @@
       <c r="E21" s="8">
         <v>1040331</v>
       </c>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>27</v>
       </c>
@@ -2617,9 +2385,8 @@
       <c r="E22" s="8">
         <v>1065190</v>
       </c>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -2635,9 +2402,8 @@
       <c r="E23" s="8">
         <v>1046485</v>
       </c>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>29</v>
       </c>
@@ -2653,9 +2419,8 @@
       <c r="E24" s="8">
         <v>1005162</v>
       </c>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
@@ -2671,9 +2436,8 @@
       <c r="E25" s="8">
         <v>1081246</v>
       </c>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>31</v>
       </c>
@@ -2689,9 +2453,8 @@
       <c r="E26" s="8">
         <v>1189057</v>
       </c>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>32</v>
       </c>
@@ -2707,9 +2470,8 @@
       <c r="E27" s="8">
         <v>1153222</v>
       </c>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>33</v>
       </c>
@@ -2725,9 +2487,8 @@
       <c r="E28" s="8">
         <v>1206487</v>
       </c>
-      <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>34</v>
       </c>
@@ -2743,9 +2504,8 @@
       <c r="E29" s="8">
         <v>1280683</v>
       </c>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>35</v>
       </c>
@@ -2761,9 +2521,8 @@
       <c r="E30" s="8">
         <v>1377447</v>
       </c>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>36</v>
       </c>
@@ -2779,9 +2538,8 @@
       <c r="E31" s="8">
         <v>1454962</v>
       </c>
-      <c r="F31" s="8"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>37</v>
       </c>
@@ -2797,9 +2555,8 @@
       <c r="E32" s="8">
         <v>1595907</v>
       </c>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>38</v>
       </c>
@@ -2815,9 +2572,8 @@
       <c r="E33" s="8">
         <v>1557060</v>
       </c>
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>39</v>
       </c>
@@ -2833,9 +2589,8 @@
       <c r="E34" s="8">
         <v>1632858</v>
       </c>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>40</v>
       </c>
@@ -2851,9 +2606,8 @@
       <c r="E35" s="8">
         <v>1703929</v>
       </c>
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>41</v>
       </c>
@@ -2869,11 +2623,10 @@
       <c r="E36" s="8">
         <v>1732058</v>
       </c>
-      <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B37" s="8">
         <v>182</v>
@@ -2887,11 +2640,10 @@
       <c r="E37" s="8">
         <v>1787673</v>
       </c>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B38" s="8">
         <v>181</v>
@@ -2905,11 +2657,10 @@
       <c r="E38" s="8">
         <v>1893368</v>
       </c>
-      <c r="F38" s="8"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B39" s="8">
         <v>177</v>
@@ -2923,11 +2674,10 @@
       <c r="E39" s="8">
         <v>1921326</v>
       </c>
-      <c r="F39" s="8"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B40" s="8">
         <v>181</v>
@@ -2941,11 +2691,10 @@
       <c r="E40" s="8">
         <v>2016366</v>
       </c>
-      <c r="F40" s="8"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B41" s="8">
         <v>180</v>
@@ -2959,11 +2708,10 @@
       <c r="E41" s="8">
         <v>2008132</v>
       </c>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B42" s="8">
         <v>180</v>
@@ -2977,11 +2725,10 @@
       <c r="E42" s="8">
         <v>2094092</v>
       </c>
-      <c r="F42" s="8"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B43" s="8">
         <v>187</v>
@@ -2995,11 +2742,10 @@
       <c r="E43" s="8">
         <v>1331929</v>
       </c>
-      <c r="F43" s="8"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B44" s="8">
         <v>185</v>
@@ -3013,11 +2759,10 @@
       <c r="E44" s="8">
         <v>1264753</v>
       </c>
-      <c r="F44" s="8"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B45" s="8">
         <v>183</v>
@@ -3031,11 +2776,10 @@
       <c r="E45" s="8">
         <v>2058917</v>
       </c>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B46" s="8">
         <v>183</v>
@@ -3049,11 +2793,10 @@
       <c r="E46" s="8">
         <v>2103510</v>
       </c>
-      <c r="F46" s="8"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B47" s="8">
         <v>182</v>
@@ -3067,11 +2810,10 @@
       <c r="E47" s="8">
         <v>2221047</v>
       </c>
-      <c r="F47" s="8"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B48" s="8">
         <v>182</v>
@@ -3085,11 +2827,10 @@
       <c r="E48" s="8">
         <v>2245960</v>
       </c>
-      <c r="F48" s="8"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B49" s="8">
         <v>181</v>
@@ -3103,11 +2844,10 @@
       <c r="E49" s="8">
         <v>2268408</v>
       </c>
-      <c r="F49" s="8"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="B50" s="8">
         <v>182</v>
@@ -3121,11 +2861,10 @@
       <c r="E50" s="8">
         <v>2317387</v>
       </c>
-      <c r="F50" s="8"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B51" s="8">
         <v>185</v>
@@ -3139,11 +2878,10 @@
       <c r="E51" s="8">
         <v>2291430</v>
       </c>
-      <c r="F51" s="8"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B52" s="8">
         <v>181</v>
@@ -3157,11 +2895,10 @@
       <c r="E52" s="8">
         <v>2387566</v>
       </c>
-      <c r="F52" s="8"/>
-    </row>
-    <row r="53" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B53" s="11">
         <v>184</v>
@@ -3175,41 +2912,54 @@
       <c r="E53" s="11">
         <v>2358917</v>
       </c>
-      <c r="F53" s="11"/>
-    </row>
-    <row r="54" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B54" s="6">
-        <v>179</v>
-      </c>
-      <c r="C54" s="13">
-        <v>354305</v>
-      </c>
-      <c r="D54" s="13">
-        <v>2360879</v>
-      </c>
-      <c r="E54" s="13">
-        <v>2335777</v>
-      </c>
-      <c r="F54" s="6"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="10">
+        <v>185</v>
+      </c>
+      <c r="C54" s="11">
+        <v>357585</v>
+      </c>
+      <c r="D54" s="11">
+        <v>2380539</v>
+      </c>
+      <c r="E54" s="11">
+        <v>2345917</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="23">
+        <v>177</v>
+      </c>
+      <c r="C55" s="23">
+        <v>353081</v>
+      </c>
+      <c r="D55" s="24">
+        <v>2368883</v>
+      </c>
+      <c r="E55" s="24">
+        <v>2348249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="23"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3219,306 +2969,271 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B2" s="7">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C2" s="8">
-        <v>338390</v>
+        <v>331055</v>
       </c>
       <c r="D2" s="8">
-        <v>1465033.7</v>
+        <v>1331534.94</v>
       </c>
       <c r="E2" s="8">
-        <v>1331929</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1264753</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C3" s="8">
-        <v>331055</v>
+        <v>335608</v>
       </c>
       <c r="D3" s="8">
-        <v>1331534.94</v>
+        <v>2129456</v>
       </c>
       <c r="E3" s="8">
-        <v>1264753</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2058917</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B4" s="7">
         <v>183</v>
       </c>
       <c r="C4" s="8">
-        <v>335608</v>
+        <v>338746</v>
       </c>
       <c r="D4" s="8">
-        <v>2129456</v>
+        <v>2248174</v>
       </c>
       <c r="E4" s="8">
-        <v>2058917</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2103510</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B5" s="7">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C5" s="8">
-        <v>338746</v>
+        <v>347237</v>
       </c>
       <c r="D5" s="8">
-        <v>2248174</v>
+        <v>2321303</v>
       </c>
       <c r="E5" s="8">
-        <v>2103510</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2221047</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B6" s="7">
         <v>182</v>
       </c>
       <c r="C6" s="8">
-        <v>347237</v>
+        <v>353577</v>
       </c>
       <c r="D6" s="8">
-        <v>2321303</v>
+        <v>2363897</v>
       </c>
       <c r="E6" s="8">
-        <v>2221047</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2245960</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B7" s="7">
+        <v>181</v>
+      </c>
+      <c r="C7" s="8">
+        <v>353411</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2372639</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2268408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="7">
         <v>182</v>
       </c>
-      <c r="C7" s="8">
-        <v>353577</v>
-      </c>
-      <c r="D7" s="8">
-        <v>2363897</v>
-      </c>
-      <c r="E7" s="8">
-        <v>2245960</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="7">
+      <c r="C8" s="8">
+        <v>353885</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2373945</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2317387</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="7">
+        <v>185</v>
+      </c>
+      <c r="C9" s="8">
+        <v>349801</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2339059.7142857141</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2291430</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="7">
         <v>181</v>
       </c>
-      <c r="C8" s="8">
-        <v>353411</v>
-      </c>
-      <c r="D8" s="8">
-        <v>2372639</v>
-      </c>
-      <c r="E8" s="8">
-        <v>2268408</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="C10" s="8">
+        <v>362962</v>
+      </c>
+      <c r="D10" s="8">
+        <v>2436410</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2387566</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="7">
+        <v>184</v>
+      </c>
+      <c r="C11" s="8">
+        <v>359285</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2389189</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2358917</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="7">
+        <v>185</v>
+      </c>
+      <c r="C12" s="8">
+        <v>357585</v>
+      </c>
+      <c r="D12" s="8">
+        <v>2380539</v>
+      </c>
+      <c r="E12" s="8">
+        <v>2345917</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="7">
-        <v>182</v>
-      </c>
-      <c r="C9" s="8">
-        <v>353885</v>
-      </c>
-      <c r="D9" s="8">
-        <v>2373945</v>
-      </c>
-      <c r="E9" s="8">
-        <v>2317387</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="7">
-        <v>185</v>
-      </c>
-      <c r="C10" s="8">
-        <v>349801</v>
-      </c>
-      <c r="D10" s="8">
-        <v>2339059.7142857141</v>
-      </c>
-      <c r="E10" s="8">
-        <v>2291430</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="7">
-        <v>181</v>
-      </c>
-      <c r="C11" s="8">
-        <v>362962</v>
-      </c>
-      <c r="D11" s="8">
-        <v>2436410</v>
-      </c>
-      <c r="E11" s="8">
-        <v>2387566</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="7">
-        <v>184</v>
-      </c>
-      <c r="C12" s="8">
-        <v>359285</v>
-      </c>
-      <c r="D12" s="8">
-        <v>2389189</v>
-      </c>
-      <c r="E12" s="8">
-        <v>2358917</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>83</v>
-      </c>
       <c r="B13" s="6">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C13" s="13">
-        <v>354305</v>
+        <v>353081</v>
       </c>
       <c r="D13" s="13">
-        <v>2360879</v>
+        <v>2368883</v>
       </c>
       <c r="E13" s="13">
-        <v>2335777</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+        <v>2348249</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4038,25 +3753,35 @@
         <v>3767</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="6">
+    <row r="49" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
         <v>37</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="10">
         <v>9</v>
       </c>
-      <c r="C49" s="13">
+      <c r="C49" s="11">
         <v>3525</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="8"/>
+    <row r="50" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>38</v>
+      </c>
+      <c r="B50" s="6">
+        <v>10</v>
+      </c>
+      <c r="C50" s="13">
+        <v>2893</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
/home/ofenloch/workspaces/COVID19/rki-data-evaluation/getRKIData.sh: add data automatically downloaded at 2021-04-22--05-03-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Testzahlen-gesamt.xlsx
+++ b/rki-data/RKI-Testzahlen-gesamt.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seifriedj\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\U3LIQEGP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9824851E-BC3E-476B-ABE7-44CD0D4E1CB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CE9A07-BB48-414F-9CE0-D66DC83F2F92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="14460" windowHeight="9650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_Erläuterungen" sheetId="7" r:id="rId1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="78">
   <si>
     <t>Das RKI erfasst wöchentlich die SARS-CoV-2-Testzahlen. Hierfür werden deutschlandweit Daten von Universitätskliniken, Forschungseinrichtungen sowie klinischen und ambulanten Laboren zusammengeführt. Die Erfassung basiert auf einer freiwilligen Mitteilung der Labore und erfolgt über eine webbasierte Plattform (VOXCO, RKI-Testlaborabfrage) oder in Zusammenarbeit mit der am RKI etablierten, laborbasierten SARS-CoV-2-Surveillance (eine Erweiterung der Antibiotika-Resistenz-Surveillance, ARS), dem Netzwerk für respiratorische Viren (RespVir) sowie der Abfrage eines labormedizinischen Berufsverbands. Die Erfassung liefert Hinweise zur aktuellen Situation in den Laboren, erlaubt aber keine detaillierten Auswertungen oder Vergleiche mit den gemeldeten Fallzahlen.</t>
   </si>
@@ -219,10 +214,13 @@
     <t>14/2021</t>
   </si>
   <si>
+    <t>15/2021</t>
+  </si>
+  <si>
     <t>Summe</t>
   </si>
   <si>
-    <t>Bis einschließlich KW4/2021</t>
+    <t>Bis einschließlich KW5/2021</t>
   </si>
   <si>
     <t>KW, für die die Angabe prognostisch erfolgt ist</t>
@@ -240,7 +238,7 @@
     <t>Reale Testkapazität zum Zeitpunkt der Abfrage</t>
   </si>
   <si>
-    <t>15/2021</t>
+    <t>16/2021</t>
   </si>
   <si>
     <t>Labore mit Rückstau</t>
@@ -313,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -351,8 +349,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -369,13 +371,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{2BAEE300-0785-409B-9ECA-EF7231A7A395}"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{FC40BBD3-355B-4913-963C-1E1AE1BA8A91}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -395,14 +394,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -410,7 +409,7 @@
         <xdr:cNvPr id="3" name="Grafik 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F59D9FB6-5876-4CF6-B5BB-1689201F3BF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AFA1BA3-D42D-4557-9AE1-6C65A1BB3F8E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -432,8 +431,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4362450" y="952500"/>
-          <a:ext cx="10058400" cy="4470400"/>
+          <a:off x="4572000" y="508000"/>
+          <a:ext cx="9772650" cy="4343400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -741,32 +740,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D570AD-7229-42F4-8853-0B48620792E3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2B9231-EB8D-4A9E-93C6-AD643485F64F}">
   <dimension ref="A3:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="140.81640625" style="5" customWidth="1"/>
-    <col min="2" max="16384" width="11.453125" style="3"/>
+    <col min="1" max="1" width="140.85546875" style="5" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" s="2" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" s="2" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="126" customHeight="1" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -777,22 +776,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -808,8 +807,9 @@
       <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -821,8 +821,9 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -838,8 +839,9 @@
       <c r="E3" s="7">
         <v>118</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -855,8 +857,9 @@
       <c r="E4" s="7">
         <v>154</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -872,8 +875,9 @@
       <c r="E5" s="7">
         <v>159</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -889,8 +893,9 @@
       <c r="E6" s="7">
         <v>163</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -906,8 +911,9 @@
       <c r="E7" s="7">
         <v>175</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -923,8 +929,9 @@
       <c r="E8" s="7">
         <v>172</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -940,8 +947,9 @@
       <c r="E9" s="7">
         <v>180</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
@@ -957,8 +965,9 @@
       <c r="E10" s="7">
         <v>178</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -974,8 +983,9 @@
       <c r="E11" s="7">
         <v>181</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -991,8 +1001,9 @@
       <c r="E12" s="7">
         <v>183</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1008,8 +1019,9 @@
       <c r="E13" s="7">
         <v>181</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
@@ -1025,8 +1037,9 @@
       <c r="E14" s="7">
         <v>175</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1042,8 +1055,9 @@
       <c r="E15" s="7">
         <v>178</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -1059,8 +1073,9 @@
       <c r="E16" s="7">
         <v>175</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
@@ -1076,8 +1091,9 @@
       <c r="E17" s="7">
         <v>175</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
@@ -1093,8 +1109,9 @@
       <c r="E18" s="7">
         <v>182</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>23</v>
       </c>
@@ -1110,8 +1127,9 @@
       <c r="E19" s="7">
         <v>154</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -1127,8 +1145,9 @@
       <c r="E20" s="7">
         <v>182</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
@@ -1144,8 +1163,9 @@
       <c r="E21" s="7">
         <v>182</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
@@ -1161,8 +1181,9 @@
       <c r="E22" s="7">
         <v>187</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
@@ -1178,8 +1199,9 @@
       <c r="E23" s="7">
         <v>175</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
@@ -1195,8 +1217,9 @@
       <c r="E24" s="7">
         <v>174</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
@@ -1212,8 +1235,9 @@
       <c r="E25" s="7">
         <v>189</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
@@ -1229,8 +1253,9 @@
       <c r="E26" s="7">
         <v>197</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
@@ -1246,8 +1271,9 @@
       <c r="E27" s="7">
         <v>196</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>32</v>
       </c>
@@ -1263,8 +1289,9 @@
       <c r="E28" s="7">
         <v>195</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>33</v>
       </c>
@@ -1280,8 +1307,9 @@
       <c r="E29" s="7">
         <v>197</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
@@ -1297,8 +1325,9 @@
       <c r="E30" s="7">
         <v>206</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>35</v>
       </c>
@@ -1314,8 +1343,9 @@
       <c r="E31" s="7">
         <v>200</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>36</v>
       </c>
@@ -1331,8 +1361,9 @@
       <c r="E32" s="7">
         <v>198</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>37</v>
       </c>
@@ -1348,8 +1379,9 @@
       <c r="E33" s="7">
         <v>198</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>38</v>
       </c>
@@ -1365,8 +1397,9 @@
       <c r="E34" s="7">
         <v>205</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>39</v>
       </c>
@@ -1382,8 +1415,9 @@
       <c r="E35" s="7">
         <v>209</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>40</v>
       </c>
@@ -1399,8 +1433,9 @@
       <c r="E36" s="7">
         <v>210</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>41</v>
       </c>
@@ -1416,8 +1451,9 @@
       <c r="E37" s="7">
         <v>208</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>42</v>
       </c>
@@ -1433,8 +1469,9 @@
       <c r="E38" s="7">
         <v>206</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>43</v>
       </c>
@@ -1450,8 +1487,9 @@
       <c r="E39" s="7">
         <v>204</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>44</v>
       </c>
@@ -1467,8 +1505,9 @@
       <c r="E40" s="7">
         <v>206</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>45</v>
       </c>
@@ -1484,8 +1523,9 @@
       <c r="E41" s="7">
         <v>208</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>46</v>
       </c>
@@ -1501,8 +1541,9 @@
       <c r="E42" s="7">
         <v>206</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>47</v>
       </c>
@@ -1518,8 +1559,9 @@
       <c r="E43" s="7">
         <v>212</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>48</v>
       </c>
@@ -1535,8 +1577,9 @@
       <c r="E44" s="7">
         <v>208</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>49</v>
       </c>
@@ -1552,8 +1595,9 @@
       <c r="E45" s="7">
         <v>205</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>50</v>
       </c>
@@ -1569,8 +1613,9 @@
       <c r="E46" s="7">
         <v>206</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>51</v>
       </c>
@@ -1586,8 +1631,9 @@
       <c r="E47" s="7">
         <v>206</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>52</v>
       </c>
@@ -1603,8 +1649,9 @@
       <c r="E48" s="7">
         <v>208</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>53</v>
       </c>
@@ -1620,8 +1667,9 @@
       <c r="E49" s="7">
         <v>208</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>54</v>
       </c>
@@ -1637,8 +1685,9 @@
       <c r="E50" s="7">
         <v>208</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>55</v>
       </c>
@@ -1654,8 +1703,9 @@
       <c r="E51" s="7">
         <v>213</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>56</v>
       </c>
@@ -1671,8 +1721,9 @@
       <c r="E52" s="10">
         <v>207</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F52" s="10"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>57</v>
       </c>
@@ -1688,59 +1739,63 @@
       <c r="E53" s="7">
         <v>210</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F53" s="10"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B54" s="11">
-        <v>1151639</v>
+        <v>1153270</v>
       </c>
       <c r="C54" s="11">
-        <v>71647</v>
+        <v>71715</v>
       </c>
       <c r="D54" s="12">
-        <v>6.2213071978284864</v>
+        <v>6.218405056925091</v>
       </c>
       <c r="E54" s="10">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+      <c r="F54" s="11"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B55" s="11">
-        <v>1278442</v>
+        <v>1280050</v>
       </c>
       <c r="C55" s="11">
-        <v>85587</v>
+        <v>85655</v>
       </c>
       <c r="D55" s="12">
-        <v>6.6946329986029864</v>
+        <v>6.6915354868950434</v>
       </c>
       <c r="E55" s="10">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+      <c r="F55" s="10"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B56" s="10">
-        <v>1365514</v>
+        <v>1367247</v>
       </c>
       <c r="C56" s="10">
-        <v>107758</v>
+        <v>107827</v>
       </c>
       <c r="D56" s="12">
-        <v>7.8913874189499342</v>
+        <v>7.8864316396378999</v>
       </c>
       <c r="E56" s="10">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+        <v>209</v>
+      </c>
+      <c r="F56" s="10"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>61</v>
       </c>
@@ -1756,53 +1811,80 @@
       <c r="E57" s="7">
         <v>206</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B58" s="8">
-        <v>1167760</v>
+        <v>1178378</v>
       </c>
       <c r="C58" s="8">
-        <v>128266</v>
+        <v>128814</v>
       </c>
       <c r="D58" s="9">
-        <v>10.983935055148319</v>
+        <v>10.931466812856316</v>
       </c>
       <c r="E58" s="7">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B59" s="8">
-        <v>1152511</v>
+        <v>1165380</v>
       </c>
       <c r="C59" s="8">
-        <v>138738</v>
+        <v>140491</v>
       </c>
       <c r="D59" s="9">
-        <v>12.037889443137637</v>
+        <v>12.05538107741681</v>
       </c>
       <c r="E59" s="7">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="F59" s="7"/>
+    </row>
+    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="13">
-        <v>52737238</v>
-      </c>
-      <c r="C60" s="13">
-        <v>3355934</v>
-      </c>
-      <c r="D60" s="9"/>
-      <c r="E60" s="7"/>
+      <c r="B60" s="11">
+        <v>1295635</v>
+      </c>
+      <c r="C60" s="11">
+        <v>160735</v>
+      </c>
+      <c r="D60" s="12">
+        <v>12.4058859169442</v>
+      </c>
+      <c r="E60" s="10">
+        <v>202</v>
+      </c>
+      <c r="F60" s="10"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" s="13">
+        <v>54061332</v>
+      </c>
+      <c r="C61" s="13">
+        <v>3519175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1815,237 +1897,237 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E13"/>
+      <selection activeCell="D13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.26953125" customWidth="1"/>
-    <col min="2" max="2" width="23.81640625" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="8">
+        <v>41870521</v>
+      </c>
+      <c r="C2" s="8">
+        <v>2484761</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1060602</v>
+      </c>
+      <c r="C3" s="8">
+        <v>67882</v>
+      </c>
+      <c r="D3" s="18">
+        <v>6.4003273612533258</v>
+      </c>
+      <c r="E3" s="19">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1103231</v>
+      </c>
+      <c r="C4" s="8">
+        <v>67379</v>
+      </c>
+      <c r="D4" s="18">
+        <v>6.1074244650485703</v>
+      </c>
+      <c r="E4" s="19">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1171798</v>
+      </c>
+      <c r="C5" s="8">
+        <v>72059</v>
+      </c>
+      <c r="D5" s="18">
+        <v>6.149438725787209</v>
+      </c>
+      <c r="E5" s="19">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1153270</v>
+      </c>
+      <c r="C6" s="8">
+        <v>71715</v>
+      </c>
+      <c r="D6" s="18">
+        <v>6.218405056925091</v>
+      </c>
+      <c r="E6" s="19">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1280050</v>
+      </c>
+      <c r="C7" s="8">
+        <v>85655</v>
+      </c>
+      <c r="D7" s="18">
+        <v>6.6915354868950434</v>
+      </c>
+      <c r="E7" s="19">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1367247</v>
+      </c>
+      <c r="C8" s="8">
+        <v>107827</v>
+      </c>
+      <c r="D8" s="18">
+        <v>7.8864316396378999</v>
+      </c>
+      <c r="E8" s="19">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1415220</v>
+      </c>
+      <c r="C9" s="8">
+        <v>131857</v>
+      </c>
+      <c r="D9" s="18">
+        <v>9.317067311089442</v>
+      </c>
+      <c r="E9" s="19">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1178378</v>
+      </c>
+      <c r="C10" s="8">
+        <v>128814</v>
+      </c>
+      <c r="D10" s="18">
+        <v>10.931466812856316</v>
+      </c>
+      <c r="E10" s="19">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1165380</v>
+      </c>
+      <c r="C11" s="8">
+        <v>140491</v>
+      </c>
+      <c r="D11" s="18">
+        <v>12.05538107741681</v>
+      </c>
+      <c r="E11" s="19">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1295635</v>
+      </c>
+      <c r="C12" s="8">
+        <v>160735</v>
+      </c>
+      <c r="D12" s="18">
+        <v>12.4058859169442</v>
+      </c>
+      <c r="E12" s="19">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="8">
-        <v>40769022</v>
-      </c>
-      <c r="C2" s="8">
-        <v>2402325</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="8">
-        <v>1101499</v>
-      </c>
-      <c r="C3" s="8">
-        <v>82436</v>
-      </c>
-      <c r="D3" s="16">
-        <v>7.4839831901799272</v>
-      </c>
-      <c r="E3" s="17">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="8">
-        <v>1060602</v>
-      </c>
-      <c r="C4" s="8">
-        <v>67882</v>
-      </c>
-      <c r="D4" s="16">
-        <v>6.4003273612533258</v>
-      </c>
-      <c r="E4" s="17">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1103231</v>
-      </c>
-      <c r="C5" s="8">
-        <v>67379</v>
-      </c>
-      <c r="D5" s="16">
-        <v>6.1074244650485703</v>
-      </c>
-      <c r="E5" s="17">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1171798</v>
-      </c>
-      <c r="C6" s="8">
-        <v>72059</v>
-      </c>
-      <c r="D6" s="16">
-        <v>6.149438725787209</v>
-      </c>
-      <c r="E6" s="17">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1151639</v>
-      </c>
-      <c r="C7" s="8">
-        <v>71647</v>
-      </c>
-      <c r="D7" s="16">
-        <v>6.2213071978284864</v>
-      </c>
-      <c r="E7" s="17">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1278442</v>
-      </c>
-      <c r="C8" s="8">
-        <v>85587</v>
-      </c>
-      <c r="D8" s="16">
-        <v>6.6946329986029864</v>
-      </c>
-      <c r="E8" s="17">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="8">
-        <v>1365514</v>
-      </c>
-      <c r="C9" s="8">
-        <v>107758</v>
-      </c>
-      <c r="D9" s="16">
-        <v>7.8913874189499342</v>
-      </c>
-      <c r="E9" s="17">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1415220</v>
-      </c>
-      <c r="C10" s="8">
-        <v>131857</v>
-      </c>
-      <c r="D10" s="16">
-        <v>9.317067311089442</v>
-      </c>
-      <c r="E10" s="17">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1167760</v>
-      </c>
-      <c r="C11" s="8">
-        <v>128266</v>
-      </c>
-      <c r="D11" s="16">
-        <v>10.983935055148319</v>
-      </c>
-      <c r="E11" s="17">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="8">
-        <v>1152511</v>
-      </c>
-      <c r="C12" s="8">
-        <v>138738</v>
-      </c>
-      <c r="D12" s="16">
-        <v>12.037889443137637</v>
-      </c>
-      <c r="E12" s="17">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>64</v>
-      </c>
       <c r="B13" s="13">
-        <v>52737238</v>
+        <v>54061332</v>
       </c>
       <c r="C13" s="13">
-        <v>3355934</v>
+        <v>3519175</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2055,41 +2137,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="99.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E1" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -2106,9 +2187,8 @@
         <v>40950</v>
       </c>
       <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -2125,9 +2205,8 @@
         <v>119700</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -2144,9 +2223,8 @@
         <v>367630</v>
       </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -2163,9 +2241,8 @@
         <v>531380</v>
       </c>
       <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
@@ -2182,9 +2259,8 @@
         <v>664960</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -2201,9 +2277,8 @@
         <v>670650</v>
       </c>
       <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -2220,9 +2295,8 @@
         <v>700399</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
@@ -2239,9 +2313,8 @@
         <v>730541</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
@@ -2258,9 +2331,8 @@
         <v>831816</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>16</v>
       </c>
@@ -2277,9 +2349,8 @@
         <v>873162</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
@@ -2296,9 +2367,8 @@
         <v>882561</v>
       </c>
       <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
@@ -2315,9 +2385,8 @@
         <v>880441</v>
       </c>
       <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>19</v>
       </c>
@@ -2334,9 +2403,8 @@
         <v>939801</v>
       </c>
       <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
@@ -2353,9 +2421,8 @@
         <v>974698</v>
       </c>
       <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>21</v>
       </c>
@@ -2372,9 +2439,8 @@
         <v>996309</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
@@ -2391,9 +2457,8 @@
         <v>994060</v>
       </c>
       <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>23</v>
       </c>
@@ -2410,9 +2475,8 @@
         <v>1003758</v>
       </c>
       <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>24</v>
       </c>
@@ -2429,9 +2493,8 @@
         <v>1020962</v>
       </c>
       <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>25</v>
       </c>
@@ -2448,9 +2511,8 @@
         <v>1041871</v>
       </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>26</v>
       </c>
@@ -2467,9 +2529,8 @@
         <v>1040331</v>
       </c>
       <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>27</v>
       </c>
@@ -2486,9 +2547,8 @@
         <v>1065190</v>
       </c>
       <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -2505,9 +2565,8 @@
         <v>1046485</v>
       </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>29</v>
       </c>
@@ -2524,9 +2583,8 @@
         <v>1005162</v>
       </c>
       <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
@@ -2543,9 +2601,8 @@
         <v>1081246</v>
       </c>
       <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>31</v>
       </c>
@@ -2562,9 +2619,8 @@
         <v>1189057</v>
       </c>
       <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>32</v>
       </c>
@@ -2581,9 +2637,8 @@
         <v>1153222</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>33</v>
       </c>
@@ -2600,9 +2655,8 @@
         <v>1206487</v>
       </c>
       <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>34</v>
       </c>
@@ -2619,9 +2673,8 @@
         <v>1280683</v>
       </c>
       <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>35</v>
       </c>
@@ -2638,9 +2691,8 @@
         <v>1377447</v>
       </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>36</v>
       </c>
@@ -2657,9 +2709,8 @@
         <v>1454962</v>
       </c>
       <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>37</v>
       </c>
@@ -2676,9 +2727,8 @@
         <v>1595907</v>
       </c>
       <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>38</v>
       </c>
@@ -2695,9 +2745,8 @@
         <v>1557060</v>
       </c>
       <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>39</v>
       </c>
@@ -2714,9 +2763,8 @@
         <v>1632858</v>
       </c>
       <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>40</v>
       </c>
@@ -2733,9 +2781,8 @@
         <v>1703929</v>
       </c>
       <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>41</v>
       </c>
@@ -2752,9 +2799,8 @@
         <v>1732058</v>
       </c>
       <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>42</v>
       </c>
@@ -2771,9 +2817,8 @@
         <v>1787673</v>
       </c>
       <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>43</v>
       </c>
@@ -2790,9 +2835,8 @@
         <v>1893368</v>
       </c>
       <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>44</v>
       </c>
@@ -2809,9 +2853,8 @@
         <v>1921326</v>
       </c>
       <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>45</v>
       </c>
@@ -2828,9 +2871,8 @@
         <v>2016366</v>
       </c>
       <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>46</v>
       </c>
@@ -2847,9 +2889,8 @@
         <v>2008132</v>
       </c>
       <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>47</v>
       </c>
@@ -2866,9 +2907,8 @@
         <v>2094092</v>
       </c>
       <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>48</v>
       </c>
@@ -2885,9 +2925,8 @@
         <v>1331929</v>
       </c>
       <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>49</v>
       </c>
@@ -2904,9 +2943,8 @@
         <v>1264753</v>
       </c>
       <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>50</v>
       </c>
@@ -2923,9 +2961,8 @@
         <v>2058917</v>
       </c>
       <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>51</v>
       </c>
@@ -2942,9 +2979,8 @@
         <v>2103510</v>
       </c>
       <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>52</v>
       </c>
@@ -2961,9 +2997,8 @@
         <v>2221047</v>
       </c>
       <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>53</v>
       </c>
@@ -2980,9 +3015,8 @@
         <v>2247760</v>
       </c>
       <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>54</v>
       </c>
@@ -2999,9 +3033,8 @@
         <v>2270208</v>
       </c>
       <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>55</v>
       </c>
@@ -3018,9 +3051,8 @@
         <v>2319187</v>
       </c>
       <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>56</v>
       </c>
@@ -3037,9 +3069,8 @@
         <v>2294630</v>
       </c>
       <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>57</v>
       </c>
@@ -3056,9 +3087,8 @@
         <v>2391466</v>
       </c>
       <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>58</v>
       </c>
@@ -3075,406 +3105,431 @@
         <v>2361017</v>
       </c>
       <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-    </row>
-    <row r="54" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="10">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C54" s="11">
-        <v>358185</v>
+        <v>358485</v>
       </c>
       <c r="D54" s="11">
-        <v>2384739</v>
+        <v>2386839</v>
       </c>
       <c r="E54" s="11">
-        <v>2345917</v>
+        <v>2348017</v>
       </c>
       <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-    </row>
-    <row r="55" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="19" t="s">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="19">
-        <v>186</v>
-      </c>
-      <c r="C55" s="19">
-        <v>360611</v>
-      </c>
-      <c r="D55" s="20">
-        <v>2412343</v>
-      </c>
-      <c r="E55" s="19">
-        <v>2384239</v>
-      </c>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B55" s="21">
+        <v>187</v>
+      </c>
+      <c r="C55" s="21">
+        <v>360911</v>
+      </c>
+      <c r="D55" s="22">
+        <v>2414443</v>
+      </c>
+      <c r="E55" s="21">
+        <v>2386339</v>
+      </c>
+      <c r="F55" s="21"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="8">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C56" s="8">
-        <v>351349</v>
+        <v>351649</v>
       </c>
       <c r="D56" s="8">
-        <v>2354103</v>
+        <v>2356203</v>
       </c>
       <c r="E56" s="8">
-        <v>2324335</v>
+        <v>2326435</v>
       </c>
       <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="19" t="s">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B57" s="20">
+      <c r="B57" s="22">
         <v>180</v>
       </c>
-      <c r="C57" s="20">
+      <c r="C57" s="22">
         <v>351313</v>
       </c>
-      <c r="D57" s="20">
+      <c r="D57" s="22">
         <v>2329923</v>
       </c>
-      <c r="E57" s="20">
+      <c r="E57" s="22">
         <v>2321963</v>
       </c>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F57" s="21"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="8">
+        <v>182</v>
+      </c>
+      <c r="C58" s="8">
+        <v>353705</v>
+      </c>
+      <c r="D58" s="8">
+        <v>2336559</v>
+      </c>
+      <c r="E58" s="8">
+        <v>2332259</v>
+      </c>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="11">
         <v>180</v>
       </c>
-      <c r="C58" s="8">
-        <v>352005</v>
-      </c>
-      <c r="D58" s="8">
-        <v>2326959</v>
-      </c>
-      <c r="E58" s="8">
-        <v>2330859</v>
-      </c>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B59" s="13">
+      <c r="C59" s="11">
+        <v>351985</v>
+      </c>
+      <c r="D59" s="11">
+        <v>2305267</v>
+      </c>
+      <c r="E59" s="11">
+        <v>2358863</v>
+      </c>
+      <c r="F59" s="13"/>
+    </row>
+    <row r="60" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" s="13">
         <v>176</v>
       </c>
-      <c r="C59" s="13">
-        <v>349105</v>
-      </c>
-      <c r="D59" s="13">
-        <v>2287807</v>
-      </c>
-      <c r="E59" s="13">
-        <v>2356923</v>
-      </c>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
+      <c r="C60" s="13">
+        <v>352811</v>
+      </c>
+      <c r="D60" s="13">
+        <v>2368413</v>
+      </c>
+      <c r="E60" s="13">
+        <v>2370981</v>
+      </c>
+      <c r="F60" s="13"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="20"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.453125" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" customWidth="1"/>
-    <col min="5" max="5" width="21.26953125" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="20" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E1" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" s="7">
+        <v>182</v>
+      </c>
+      <c r="C2" s="8">
+        <v>354011</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2376839</v>
+      </c>
+      <c r="E2" s="8">
+        <v>2270208</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7">
         <v>183</v>
       </c>
-      <c r="C2" s="8">
-        <v>354177</v>
-      </c>
-      <c r="D2" s="8">
-        <v>2368097</v>
-      </c>
-      <c r="E2" s="8">
-        <v>2247760</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="7">
+      <c r="C3" s="8">
+        <v>354485</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2378145</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2319187</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="7">
+        <v>187</v>
+      </c>
+      <c r="C4" s="8">
+        <v>350601</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2344259.7142857141</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2294630</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="7">
+        <v>183</v>
+      </c>
+      <c r="C5" s="8">
+        <v>363862</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2442710</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2391466</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="7">
+        <v>185</v>
+      </c>
+      <c r="C6" s="8">
+        <v>359585</v>
+      </c>
+      <c r="D6" s="8">
+        <v>2391289</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2361017</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="7">
+        <v>187</v>
+      </c>
+      <c r="C7" s="8">
+        <v>358485</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2386839</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2348017</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="7">
+        <v>187</v>
+      </c>
+      <c r="C8" s="8">
+        <v>360911</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2414443</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2386339</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="7">
         <v>182</v>
       </c>
-      <c r="C3" s="8">
-        <v>354011</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2376839</v>
-      </c>
-      <c r="E3" s="8">
-        <v>2270208</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="7">
-        <v>183</v>
-      </c>
-      <c r="C4" s="8">
-        <v>354485</v>
-      </c>
-      <c r="D4" s="8">
-        <v>2378145</v>
-      </c>
-      <c r="E4" s="8">
-        <v>2319187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="7">
-        <v>187</v>
-      </c>
-      <c r="C5" s="8">
-        <v>350601</v>
-      </c>
-      <c r="D5" s="8">
-        <v>2344259.7142857141</v>
-      </c>
-      <c r="E5" s="8">
-        <v>2294630</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="7">
-        <v>183</v>
-      </c>
-      <c r="C6" s="8">
-        <v>363862</v>
-      </c>
-      <c r="D6" s="8">
-        <v>2442710</v>
-      </c>
-      <c r="E6" s="8">
-        <v>2391466</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="7">
-        <v>185</v>
-      </c>
-      <c r="C7" s="8">
-        <v>359585</v>
-      </c>
-      <c r="D7" s="8">
-        <v>2391289</v>
-      </c>
-      <c r="E7" s="8">
-        <v>2361017</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="7">
-        <v>186</v>
-      </c>
-      <c r="C8" s="8">
-        <v>358185</v>
-      </c>
-      <c r="D8" s="8">
-        <v>2384739</v>
-      </c>
-      <c r="E8" s="8">
-        <v>2345917</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="7">
-        <v>186</v>
-      </c>
       <c r="C9" s="8">
-        <v>360611</v>
+        <v>351649</v>
       </c>
       <c r="D9" s="8">
-        <v>2412343</v>
+        <v>2356203</v>
       </c>
       <c r="E9" s="8">
-        <v>2384239</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2326435</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" s="7">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C10" s="8">
-        <v>351349</v>
+        <v>351313</v>
       </c>
       <c r="D10" s="8">
-        <v>2354103</v>
+        <v>2329923</v>
       </c>
       <c r="E10" s="8">
-        <v>2324335</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2321963</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B11" s="7">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C11" s="8">
-        <v>351313</v>
+        <v>353705</v>
       </c>
       <c r="D11" s="8">
-        <v>2329923</v>
+        <v>2336559</v>
       </c>
       <c r="E11" s="8">
-        <v>2321963</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2332259</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" s="7">
         <v>180</v>
       </c>
       <c r="C12" s="8">
-        <v>352005</v>
+        <v>351985</v>
       </c>
       <c r="D12" s="8">
-        <v>2326959</v>
+        <v>2305267</v>
       </c>
       <c r="E12" s="8">
-        <v>2330859</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2358863</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B13" s="6">
         <v>176</v>
       </c>
       <c r="C13" s="13">
-        <v>349105</v>
+        <v>352811</v>
       </c>
       <c r="D13" s="13">
-        <v>2287807</v>
+        <v>2368413</v>
       </c>
       <c r="E13" s="13">
-        <v>2356923</v>
-      </c>
+        <v>2370981</v>
+      </c>
+      <c r="F13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="20.54296875" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>24</v>
       </c>
@@ -3485,7 +3540,7 @@
         <v>3423</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>35</v>
       </c>
@@ -3496,7 +3551,7 @@
         <v>2259</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>28</v>
       </c>
@@ -3507,7 +3562,7 @@
         <v>2243</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>30</v>
       </c>
@@ -3518,7 +3573,7 @@
         <v>3790</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>29</v>
       </c>
@@ -3529,7 +3584,7 @@
         <v>3224</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>29</v>
       </c>
@@ -3540,7 +3595,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>29</v>
       </c>
@@ -3551,7 +3606,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>26</v>
       </c>
@@ -3562,7 +3617,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>27</v>
       </c>
@@ -3573,7 +3628,7 @@
         <v>2478</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>27</v>
       </c>
@@ -3584,7 +3639,7 @@
         <v>1646</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>22</v>
       </c>
@@ -3595,7 +3650,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>31</v>
       </c>
@@ -3606,7 +3661,7 @@
         <v>3056</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>21</v>
       </c>
@@ -3617,7 +3672,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>25</v>
       </c>
@@ -3628,7 +3683,7 @@
         <v>3242</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>22</v>
       </c>
@@ -3639,7 +3694,7 @@
         <v>1483</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>20</v>
       </c>
@@ -3650,7 +3705,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>24</v>
       </c>
@@ -3661,7 +3716,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>35</v>
       </c>
@@ -3672,7 +3727,7 @@
         <v>10693</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>44</v>
       </c>
@@ -3683,7 +3738,7 @@
         <v>17143</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>48</v>
       </c>
@@ -3694,7 +3749,7 @@
         <v>27828</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>49</v>
       </c>
@@ -3705,7 +3760,7 @@
         <v>36812</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>47</v>
       </c>
@@ -3716,7 +3771,7 @@
         <v>29964</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>51</v>
       </c>
@@ -3727,7 +3782,7 @@
         <v>32397</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>42</v>
       </c>
@@ -3738,7 +3793,7 @@
         <v>12617</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>46</v>
       </c>
@@ -3749,7 +3804,7 @@
         <v>15983</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>42</v>
       </c>
@@ -3760,7 +3815,7 @@
         <v>8245</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>46</v>
       </c>
@@ -3771,7 +3826,7 @@
         <v>16829</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>52</v>
       </c>
@@ -3782,7 +3837,7 @@
         <v>20799</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>57</v>
       </c>
@@ -3793,7 +3848,7 @@
         <v>69524</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>69</v>
       </c>
@@ -3804,7 +3859,7 @@
         <v>98931</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>66</v>
       </c>
@@ -3815,7 +3870,7 @@
         <v>60113</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>59</v>
       </c>
@@ -3826,7 +3881,7 @@
         <v>23780</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>50</v>
       </c>
@@ -3837,7 +3892,7 @@
         <v>17207</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>54</v>
       </c>
@@ -3848,7 +3903,7 @@
         <v>14191</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>51</v>
       </c>
@@ -3859,7 +3914,7 @@
         <v>12267</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>51</v>
       </c>
@@ -3870,7 +3925,7 @@
         <v>19159</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>57</v>
       </c>
@@ -3881,7 +3936,7 @@
         <v>21364</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>43</v>
       </c>
@@ -3892,7 +3947,7 @@
         <v>11321</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -3903,7 +3958,7 @@
         <v>6507</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>47</v>
       </c>
@@ -3914,7 +3969,7 @@
         <v>11691</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>46</v>
       </c>
@@ -3925,7 +3980,7 @@
         <v>11336</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>48</v>
       </c>
@@ -3936,7 +3991,7 @@
         <v>11980</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>42</v>
       </c>
@@ -3947,7 +4002,7 @@
         <v>5572</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>42</v>
       </c>
@@ -3958,7 +4013,7 @@
         <v>6202</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>46</v>
       </c>
@@ -3969,7 +4024,7 @@
         <v>5850</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>44</v>
       </c>
@@ -3980,7 +4035,7 @@
         <v>6820</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>44</v>
       </c>
@@ -3991,7 +4046,7 @@
         <v>3767</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>37</v>
       </c>
@@ -4002,7 +4057,7 @@
         <v>3525</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>38</v>
       </c>
@@ -4013,7 +4068,7 @@
         <v>2893</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>43</v>
       </c>
@@ -4024,7 +4079,7 @@
         <v>4766</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>39</v>
       </c>
@@ -4035,7 +4090,7 @@
         <v>8033</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>31</v>
       </c>
@@ -4046,19 +4101,36 @@
         <v>2527</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="6">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="10">
         <v>44</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="10">
         <v>14</v>
       </c>
-      <c r="C54" s="13">
+      <c r="C54" s="11">
         <v>3631</v>
       </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>40</v>
+      </c>
+      <c r="B55" s="6">
+        <v>15</v>
+      </c>
+      <c r="C55" s="13">
+        <v>4205</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
/home/ofenloch/workspaces/COVID19/rki-data-evaluation/getRKIData.sh: add data automatically downloaded at 2021-04-29--05-03-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Testzahlen-gesamt.xlsx
+++ b/rki-data/RKI-Testzahlen-gesamt.xlsx
@@ -2,10 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CE9A07-BB48-414F-9CE0-D66DC83F2F92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\4.6.Laborergebnisse\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9511F1F-2764-444D-AD57-71E78FD46D3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12360" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_Erläuterungen" sheetId="7" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="79">
   <si>
     <t>Das RKI erfasst wöchentlich die SARS-CoV-2-Testzahlen. Hierfür werden deutschlandweit Daten von Universitätskliniken, Forschungseinrichtungen sowie klinischen und ambulanten Laboren zusammengeführt. Die Erfassung basiert auf einer freiwilligen Mitteilung der Labore und erfolgt über eine webbasierte Plattform (VOXCO, RKI-Testlaborabfrage) oder in Zusammenarbeit mit der am RKI etablierten, laborbasierten SARS-CoV-2-Surveillance (eine Erweiterung der Antibiotika-Resistenz-Surveillance, ARS), dem Netzwerk für respiratorische Viren (RespVir) sowie der Abfrage eines labormedizinischen Berufsverbands. Die Erfassung liefert Hinweise zur aktuellen Situation in den Laboren, erlaubt aber keine detaillierten Auswertungen oder Vergleiche mit den gemeldeten Fallzahlen.</t>
   </si>
@@ -217,10 +222,13 @@
     <t>15/2021</t>
   </si>
   <si>
+    <t>16/2021</t>
+  </si>
+  <si>
     <t>Summe</t>
   </si>
   <si>
-    <t>Bis einschließlich KW5/2021</t>
+    <t>Bis einschließlich KW6/2021</t>
   </si>
   <si>
     <t>KW, für die die Angabe prognostisch erfolgt ist</t>
@@ -235,10 +243,7 @@
     <t>Theoretische wöchentliche Kapazität anhand von Wochenarbeitstagen</t>
   </si>
   <si>
-    <t>Reale Testkapazität zum Zeitpunkt der Abfrage</t>
-  </si>
-  <si>
-    <t>16/2021</t>
+    <t>17/2021</t>
   </si>
   <si>
     <t>Labore mit Rückstau</t>
@@ -254,6 +259,9 @@
   </si>
   <si>
     <t xml:space="preserve">Zusätzlich zur Anzahl durchgeführter Tests werden in der RKI-Testlaborabfrage und durch einen labormedizinischen Berufsverband Angaben zur täglichen (aktuellen) Testkapazität, zur Reichweite sowie zu möglichen Probenrückstaus befragt. Die Reichweite gibt an, wie viele Arbeitstage ein Labor unter Vollauslastung  der angegebenen maximalen Testkapazität unter Berücksichtigung aller notwendigen Ressourcen (Entnahmematerial, Testreagenzien, Personal u. a.) zum Zeitpunkt der Abfrage arbeiten kann. Da die Reichweite stark  vom Vorhandensein von Testreagenzien abhängig ist, stellt die Angabe eine Momentaufnahme in einem dynamischen System dar (s. Testkapazitäten, Probenrückstau). </t>
+  </si>
+  <si>
+    <t>Reale wöchentliche Testkapazität zum Zeitpunkt der Abfrage</t>
   </si>
 </sst>
 </file>
@@ -311,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -348,16 +356,14 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,10 +377,13 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{FC40BBD3-355B-4913-963C-1E1AE1BA8A91}"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{C051C6BA-6BD4-4173-9F55-7EDD80A7DD2A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -394,14 +403,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -409,7 +418,7 @@
         <xdr:cNvPr id="3" name="Grafik 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AFA1BA3-D42D-4557-9AE1-6C65A1BB3F8E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40DD20C6-0D02-4A85-B349-A75041BED636}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -431,8 +440,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4572000" y="508000"/>
-          <a:ext cx="9772650" cy="4343400"/>
+          <a:off x="4476750" y="762000"/>
+          <a:ext cx="10058400" cy="4470400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -740,11 +749,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2B9231-EB8D-4A9E-93C6-AD643485F64F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{226BCFE1-5443-4369-BB78-0CB85A269F38}">
   <dimension ref="A3:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,22 +785,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -808,8 +817,9 @@
         <v>5</v>
       </c>
       <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -822,8 +832,9 @@
       <c r="D2" s="9"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -840,8 +851,9 @@
         <v>118</v>
       </c>
       <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -858,8 +870,9 @@
         <v>154</v>
       </c>
       <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -876,8 +889,9 @@
         <v>159</v>
       </c>
       <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -894,8 +908,9 @@
         <v>163</v>
       </c>
       <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -912,8 +927,9 @@
         <v>175</v>
       </c>
       <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -930,8 +946,9 @@
         <v>172</v>
       </c>
       <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -948,8 +965,9 @@
         <v>180</v>
       </c>
       <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
@@ -966,8 +984,9 @@
         <v>178</v>
       </c>
       <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -984,8 +1003,9 @@
         <v>181</v>
       </c>
       <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -1002,8 +1022,9 @@
         <v>183</v>
       </c>
       <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1020,8 +1041,9 @@
         <v>181</v>
       </c>
       <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
@@ -1038,8 +1060,9 @@
         <v>175</v>
       </c>
       <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1056,8 +1079,9 @@
         <v>178</v>
       </c>
       <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -1074,8 +1098,9 @@
         <v>175</v>
       </c>
       <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
@@ -1092,8 +1117,9 @@
         <v>175</v>
       </c>
       <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
@@ -1110,8 +1136,9 @@
         <v>182</v>
       </c>
       <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>23</v>
       </c>
@@ -1128,8 +1155,9 @@
         <v>154</v>
       </c>
       <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -1146,8 +1174,9 @@
         <v>182</v>
       </c>
       <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
@@ -1164,8 +1193,9 @@
         <v>182</v>
       </c>
       <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
@@ -1182,8 +1212,9 @@
         <v>187</v>
       </c>
       <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
@@ -1200,8 +1231,9 @@
         <v>175</v>
       </c>
       <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
@@ -1218,8 +1250,9 @@
         <v>174</v>
       </c>
       <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
@@ -1236,8 +1269,9 @@
         <v>189</v>
       </c>
       <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
@@ -1254,8 +1288,9 @@
         <v>197</v>
       </c>
       <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
@@ -1272,8 +1307,9 @@
         <v>196</v>
       </c>
       <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>32</v>
       </c>
@@ -1290,8 +1326,9 @@
         <v>195</v>
       </c>
       <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>33</v>
       </c>
@@ -1308,8 +1345,9 @@
         <v>197</v>
       </c>
       <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
@@ -1326,8 +1364,9 @@
         <v>206</v>
       </c>
       <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>35</v>
       </c>
@@ -1344,8 +1383,9 @@
         <v>200</v>
       </c>
       <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>36</v>
       </c>
@@ -1362,8 +1402,9 @@
         <v>198</v>
       </c>
       <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>37</v>
       </c>
@@ -1380,8 +1421,9 @@
         <v>198</v>
       </c>
       <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>38</v>
       </c>
@@ -1398,8 +1440,9 @@
         <v>205</v>
       </c>
       <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>39</v>
       </c>
@@ -1416,8 +1459,9 @@
         <v>209</v>
       </c>
       <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="8"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>40</v>
       </c>
@@ -1434,8 +1478,9 @@
         <v>210</v>
       </c>
       <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>41</v>
       </c>
@@ -1452,8 +1497,9 @@
         <v>208</v>
       </c>
       <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>42</v>
       </c>
@@ -1470,8 +1516,9 @@
         <v>206</v>
       </c>
       <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>43</v>
       </c>
@@ -1488,8 +1535,9 @@
         <v>204</v>
       </c>
       <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>44</v>
       </c>
@@ -1506,8 +1554,9 @@
         <v>206</v>
       </c>
       <c r="F40" s="7"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>45</v>
       </c>
@@ -1524,8 +1573,9 @@
         <v>208</v>
       </c>
       <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>46</v>
       </c>
@@ -1542,8 +1592,9 @@
         <v>206</v>
       </c>
       <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>47</v>
       </c>
@@ -1560,8 +1611,9 @@
         <v>212</v>
       </c>
       <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>48</v>
       </c>
@@ -1578,8 +1630,9 @@
         <v>208</v>
       </c>
       <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>49</v>
       </c>
@@ -1596,8 +1649,9 @@
         <v>205</v>
       </c>
       <c r="F45" s="7"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>50</v>
       </c>
@@ -1614,8 +1668,9 @@
         <v>206</v>
       </c>
       <c r="F46" s="7"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>51</v>
       </c>
@@ -1632,8 +1687,9 @@
         <v>206</v>
       </c>
       <c r="F47" s="7"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>52</v>
       </c>
@@ -1650,8 +1706,9 @@
         <v>208</v>
       </c>
       <c r="F48" s="7"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>53</v>
       </c>
@@ -1668,8 +1725,9 @@
         <v>208</v>
       </c>
       <c r="F49" s="7"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>54</v>
       </c>
@@ -1686,8 +1744,9 @@
         <v>208</v>
       </c>
       <c r="F50" s="7"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>55</v>
       </c>
@@ -1704,8 +1763,9 @@
         <v>213</v>
       </c>
       <c r="F51" s="7"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>56</v>
       </c>
@@ -1722,8 +1782,9 @@
         <v>207</v>
       </c>
       <c r="F52" s="10"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>57</v>
       </c>
@@ -1740,8 +1801,9 @@
         <v>210</v>
       </c>
       <c r="F53" s="10"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="11"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>58</v>
       </c>
@@ -1758,8 +1820,9 @@
         <v>211</v>
       </c>
       <c r="F54" s="11"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>59</v>
       </c>
@@ -1776,8 +1839,9 @@
         <v>215</v>
       </c>
       <c r="F55" s="10"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="11"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>60</v>
       </c>
@@ -1794,8 +1858,9 @@
         <v>209</v>
       </c>
       <c r="F56" s="10"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="10"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>61</v>
       </c>
@@ -1812,8 +1877,9 @@
         <v>206</v>
       </c>
       <c r="F57" s="7"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="8"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>62</v>
       </c>
@@ -1830,61 +1896,97 @@
         <v>207</v>
       </c>
       <c r="F58" s="7"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B59" s="8">
-        <v>1165380</v>
+        <v>1168950</v>
       </c>
       <c r="C59" s="8">
-        <v>140491</v>
+        <v>140800</v>
       </c>
       <c r="D59" s="9">
-        <v>12.05538107741681</v>
+        <v>12.044997647461397</v>
       </c>
       <c r="E59" s="7">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F59" s="7"/>
-    </row>
-    <row r="60" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G59" s="8"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B60" s="11">
-        <v>1295635</v>
+        <v>1311887</v>
       </c>
       <c r="C60" s="11">
-        <v>160735</v>
+        <v>163282</v>
       </c>
       <c r="D60" s="12">
-        <v>12.4058859169442</v>
+        <v>12.446346369771177</v>
       </c>
       <c r="E60" s="10">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F60" s="10"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="G60" s="11"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="13">
-        <v>54061332</v>
-      </c>
-      <c r="C61" s="13">
-        <v>3519175</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
+      <c r="B61" s="11">
+        <v>1409259</v>
+      </c>
+      <c r="C61" s="11">
+        <v>175711</v>
+      </c>
+      <c r="D61" s="14">
+        <v>12.46832555264859</v>
+      </c>
+      <c r="E61" s="8">
+        <v>201</v>
+      </c>
+      <c r="F61" s="6"/>
+      <c r="G61" s="13"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="13">
+        <v>55490413</v>
+      </c>
+      <c r="C62" s="13">
+        <v>3697742</v>
+      </c>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1894,244 +1996,321 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E13"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="8">
+        <v>42931123</v>
+      </c>
+      <c r="C2" s="8">
+        <v>2552643</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1103231</v>
+      </c>
+      <c r="C3" s="8">
+        <v>67379</v>
+      </c>
+      <c r="D3" s="14">
+        <v>6.1074244650485703</v>
+      </c>
+      <c r="E3" s="17">
+        <v>207</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1171798</v>
+      </c>
+      <c r="C4" s="8">
+        <v>72059</v>
+      </c>
+      <c r="D4" s="14">
+        <v>6.149438725787209</v>
+      </c>
+      <c r="E4" s="17">
+        <v>210</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1153270</v>
+      </c>
+      <c r="C5" s="8">
+        <v>71715</v>
+      </c>
+      <c r="D5" s="14">
+        <v>6.218405056925091</v>
+      </c>
+      <c r="E5" s="17">
+        <v>211</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1280050</v>
+      </c>
+      <c r="C6" s="8">
+        <v>85655</v>
+      </c>
+      <c r="D6" s="14">
+        <v>6.6915354868950434</v>
+      </c>
+      <c r="E6" s="17">
+        <v>215</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1367247</v>
+      </c>
+      <c r="C7" s="8">
+        <v>107827</v>
+      </c>
+      <c r="D7" s="14">
+        <v>7.8864316396378999</v>
+      </c>
+      <c r="E7" s="17">
+        <v>209</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1415220</v>
+      </c>
+      <c r="C8" s="8">
+        <v>131857</v>
+      </c>
+      <c r="D8" s="14">
+        <v>9.317067311089442</v>
+      </c>
+      <c r="E8" s="17">
+        <v>206</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1178378</v>
+      </c>
+      <c r="C9" s="8">
+        <v>128814</v>
+      </c>
+      <c r="D9" s="14">
+        <v>10.931466812856316</v>
+      </c>
+      <c r="E9" s="17">
+        <v>207</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1168950</v>
+      </c>
+      <c r="C10" s="8">
+        <v>140800</v>
+      </c>
+      <c r="D10" s="14">
+        <v>12.044997647461397</v>
+      </c>
+      <c r="E10" s="17">
+        <v>208</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1311887</v>
+      </c>
+      <c r="C11" s="8">
+        <v>163282</v>
+      </c>
+      <c r="D11" s="14">
+        <v>12.446346369771177</v>
+      </c>
+      <c r="E11" s="17">
+        <v>208</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1409259</v>
+      </c>
+      <c r="C12" s="8">
+        <v>175711</v>
+      </c>
+      <c r="D12" s="14">
+        <v>12.46832555264859</v>
+      </c>
+      <c r="E12" s="17">
+        <v>201</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="8">
-        <v>41870521</v>
-      </c>
-      <c r="C2" s="8">
-        <v>2484761</v>
-      </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="8">
-        <v>1060602</v>
-      </c>
-      <c r="C3" s="8">
-        <v>67882</v>
-      </c>
-      <c r="D3" s="18">
-        <v>6.4003273612533258</v>
-      </c>
-      <c r="E3" s="19">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="8">
-        <v>1103231</v>
-      </c>
-      <c r="C4" s="8">
-        <v>67379</v>
-      </c>
-      <c r="D4" s="18">
-        <v>6.1074244650485703</v>
-      </c>
-      <c r="E4" s="19">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1171798</v>
-      </c>
-      <c r="C5" s="8">
-        <v>72059</v>
-      </c>
-      <c r="D5" s="18">
-        <v>6.149438725787209</v>
-      </c>
-      <c r="E5" s="19">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1153270</v>
-      </c>
-      <c r="C6" s="8">
-        <v>71715</v>
-      </c>
-      <c r="D6" s="18">
-        <v>6.218405056925091</v>
-      </c>
-      <c r="E6" s="19">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1280050</v>
-      </c>
-      <c r="C7" s="8">
-        <v>85655</v>
-      </c>
-      <c r="D7" s="18">
-        <v>6.6915354868950434</v>
-      </c>
-      <c r="E7" s="19">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1367247</v>
-      </c>
-      <c r="C8" s="8">
-        <v>107827</v>
-      </c>
-      <c r="D8" s="18">
-        <v>7.8864316396378999</v>
-      </c>
-      <c r="E8" s="19">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="8">
-        <v>1415220</v>
-      </c>
-      <c r="C9" s="8">
-        <v>131857</v>
-      </c>
-      <c r="D9" s="18">
-        <v>9.317067311089442</v>
-      </c>
-      <c r="E9" s="19">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="8">
-        <v>1178378</v>
-      </c>
-      <c r="C10" s="8">
-        <v>128814</v>
-      </c>
-      <c r="D10" s="18">
-        <v>10.931466812856316</v>
-      </c>
-      <c r="E10" s="19">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1165380</v>
-      </c>
-      <c r="C11" s="8">
-        <v>140491</v>
-      </c>
-      <c r="D11" s="18">
-        <v>12.05538107741681</v>
-      </c>
-      <c r="E11" s="19">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="8">
-        <v>1295635</v>
-      </c>
-      <c r="C12" s="8">
-        <v>160735</v>
-      </c>
-      <c r="D12" s="18">
-        <v>12.4058859169442</v>
-      </c>
-      <c r="E12" s="19">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>65</v>
-      </c>
       <c r="B13" s="13">
-        <v>54061332</v>
+        <v>55490413</v>
       </c>
       <c r="C13" s="13">
-        <v>3519175</v>
+        <v>3697742</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2139,36 +2318,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="20"/>
+      <c r="E1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -2184,7 +2363,7 @@
         <v>80300</v>
       </c>
       <c r="E2" s="8">
-        <v>40950</v>
+        <v>39000</v>
       </c>
       <c r="F2" s="8"/>
     </row>
@@ -2202,7 +2381,7 @@
         <v>164050</v>
       </c>
       <c r="E3" s="8">
-        <v>119700</v>
+        <v>117750</v>
       </c>
       <c r="F3" s="8"/>
     </row>
@@ -2220,7 +2399,7 @@
         <v>149820</v>
       </c>
       <c r="E4" s="8">
-        <v>367630</v>
+        <v>128000</v>
       </c>
       <c r="F4" s="8"/>
     </row>
@@ -2238,7 +2417,7 @@
         <v>165960</v>
       </c>
       <c r="E5" s="8">
-        <v>531380</v>
+        <v>136660</v>
       </c>
       <c r="F5" s="8"/>
     </row>
@@ -2256,7 +2435,7 @@
         <v>375420</v>
       </c>
       <c r="E6" s="8">
-        <v>664960</v>
+        <v>259650</v>
       </c>
       <c r="F6" s="8"/>
     </row>
@@ -2274,7 +2453,7 @@
         <v>831046</v>
       </c>
       <c r="E7" s="8">
-        <v>670650</v>
+        <v>589620</v>
       </c>
       <c r="F7" s="8"/>
     </row>
@@ -2292,7 +2471,7 @@
         <v>901595</v>
       </c>
       <c r="E8" s="8">
-        <v>700399</v>
+        <v>667170</v>
       </c>
       <c r="F8" s="8"/>
     </row>
@@ -2310,7 +2489,7 @@
         <v>955891</v>
       </c>
       <c r="E9" s="8">
-        <v>730541</v>
+        <v>701268</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -2328,7 +2507,7 @@
         <v>981515.00199999998</v>
       </c>
       <c r="E10" s="8">
-        <v>831816</v>
+        <v>777476</v>
       </c>
       <c r="F10" s="8"/>
     </row>
@@ -2346,7 +2525,7 @@
         <v>1030122.5</v>
       </c>
       <c r="E11" s="8">
-        <v>873162</v>
+        <v>825063</v>
       </c>
       <c r="F11" s="8"/>
     </row>
@@ -2364,7 +2543,7 @@
         <v>1057365.5</v>
       </c>
       <c r="E12" s="8">
-        <v>882561</v>
+        <v>837380</v>
       </c>
       <c r="F12" s="8"/>
     </row>
@@ -2382,7 +2561,7 @@
         <v>1033129</v>
       </c>
       <c r="E13" s="8">
-        <v>880441</v>
+        <v>821554</v>
       </c>
       <c r="F13" s="8"/>
     </row>
@@ -2400,7 +2579,7 @@
         <v>1115162.5</v>
       </c>
       <c r="E14" s="8">
-        <v>939801</v>
+        <v>904760</v>
       </c>
       <c r="F14" s="8"/>
     </row>
@@ -2418,7 +2597,7 @@
         <v>1096075</v>
       </c>
       <c r="E15" s="8">
-        <v>974698</v>
+        <v>907022</v>
       </c>
       <c r="F15" s="8"/>
     </row>
@@ -2436,7 +2615,7 @@
         <v>1123147.5</v>
       </c>
       <c r="E16" s="8">
-        <v>996309</v>
+        <v>951456</v>
       </c>
       <c r="F16" s="8"/>
     </row>
@@ -2454,7 +2633,7 @@
         <v>1131748</v>
       </c>
       <c r="E17" s="8">
-        <v>994060</v>
+        <v>950136</v>
       </c>
       <c r="F17" s="8"/>
     </row>
@@ -2472,7 +2651,7 @@
         <v>1120015</v>
       </c>
       <c r="E18" s="8">
-        <v>1003758</v>
+        <v>961246</v>
       </c>
       <c r="F18" s="8"/>
     </row>
@@ -2490,7 +2669,7 @@
         <v>1196640.0000100001</v>
       </c>
       <c r="E19" s="8">
-        <v>1020962</v>
+        <v>989576</v>
       </c>
       <c r="F19" s="8"/>
     </row>
@@ -2508,7 +2687,7 @@
         <v>1202855</v>
       </c>
       <c r="E20" s="8">
-        <v>1041871</v>
+        <v>1011165</v>
       </c>
       <c r="F20" s="8"/>
     </row>
@@ -2526,7 +2705,7 @@
         <v>1218086</v>
       </c>
       <c r="E21" s="8">
-        <v>1040331</v>
+        <v>1009137</v>
       </c>
       <c r="F21" s="8"/>
     </row>
@@ -2544,7 +2723,7 @@
         <v>1214556</v>
       </c>
       <c r="E22" s="8">
-        <v>1065190</v>
+        <v>1029124</v>
       </c>
       <c r="F22" s="8"/>
     </row>
@@ -2562,7 +2741,7 @@
         <v>1200692</v>
       </c>
       <c r="E23" s="8">
-        <v>1046485</v>
+        <v>1009346</v>
       </c>
       <c r="F23" s="8"/>
     </row>
@@ -2580,7 +2759,7 @@
         <v>1252357</v>
       </c>
       <c r="E24" s="8">
-        <v>1005162</v>
+        <v>976187</v>
       </c>
       <c r="F24" s="8"/>
     </row>
@@ -2598,7 +2777,7 @@
         <v>1308423</v>
       </c>
       <c r="E25" s="8">
-        <v>1081246</v>
+        <v>1035958</v>
       </c>
       <c r="F25" s="8"/>
     </row>
@@ -2616,7 +2795,7 @@
         <v>1362883</v>
       </c>
       <c r="E26" s="8">
-        <v>1189057</v>
+        <v>1126195</v>
       </c>
       <c r="F26" s="8"/>
     </row>
@@ -2634,7 +2813,7 @@
         <v>1376233</v>
       </c>
       <c r="E27" s="8">
-        <v>1153222</v>
+        <v>1089353</v>
       </c>
       <c r="F27" s="8"/>
     </row>
@@ -2652,7 +2831,7 @@
         <v>1458751</v>
       </c>
       <c r="E28" s="8">
-        <v>1206487</v>
+        <v>1130813</v>
       </c>
       <c r="F28" s="8"/>
     </row>
@@ -2670,7 +2849,7 @@
         <v>1512155</v>
       </c>
       <c r="E29" s="8">
-        <v>1280683</v>
+        <v>1206181</v>
       </c>
       <c r="F29" s="8"/>
     </row>
@@ -2688,7 +2867,7 @@
         <v>1540049</v>
       </c>
       <c r="E30" s="8">
-        <v>1377447</v>
+        <v>1292743</v>
       </c>
       <c r="F30" s="8"/>
     </row>
@@ -2706,7 +2885,7 @@
         <v>1564437</v>
       </c>
       <c r="E31" s="8">
-        <v>1454962</v>
+        <v>1378063</v>
       </c>
       <c r="F31" s="8"/>
     </row>
@@ -2724,7 +2903,7 @@
         <v>1705581</v>
       </c>
       <c r="E32" s="8">
-        <v>1595907</v>
+        <v>1527677</v>
       </c>
       <c r="F32" s="8"/>
     </row>
@@ -2742,7 +2921,7 @@
         <v>1700116</v>
       </c>
       <c r="E33" s="8">
-        <v>1557060</v>
+        <v>1505312</v>
       </c>
       <c r="F33" s="8"/>
     </row>
@@ -2760,7 +2939,7 @@
         <v>1790564</v>
       </c>
       <c r="E34" s="8">
-        <v>1632858</v>
+        <v>1578454</v>
       </c>
       <c r="F34" s="8"/>
     </row>
@@ -2778,7 +2957,7 @@
         <v>1910486</v>
       </c>
       <c r="E35" s="8">
-        <v>1703929</v>
+        <v>1648626</v>
       </c>
       <c r="F35" s="8"/>
     </row>
@@ -2796,7 +2975,7 @@
         <v>1937312</v>
       </c>
       <c r="E36" s="8">
-        <v>1732058</v>
+        <v>1622662</v>
       </c>
       <c r="F36" s="8"/>
     </row>
@@ -2814,7 +2993,7 @@
         <v>2020253</v>
       </c>
       <c r="E37" s="8">
-        <v>1787673</v>
+        <v>1710271</v>
       </c>
       <c r="F37" s="8"/>
     </row>
@@ -2832,7 +3011,7 @@
         <v>2079778</v>
       </c>
       <c r="E38" s="8">
-        <v>1893368</v>
+        <v>1821960</v>
       </c>
       <c r="F38" s="8"/>
     </row>
@@ -2850,7 +3029,7 @@
         <v>2141208</v>
       </c>
       <c r="E39" s="8">
-        <v>1921326</v>
+        <v>1868184</v>
       </c>
       <c r="F39" s="8"/>
     </row>
@@ -2868,7 +3047,7 @@
         <v>2202408</v>
       </c>
       <c r="E40" s="8">
-        <v>2016366</v>
+        <v>1958814</v>
       </c>
       <c r="F40" s="8"/>
     </row>
@@ -2886,7 +3065,7 @@
         <v>2235788</v>
       </c>
       <c r="E41" s="8">
-        <v>2008132</v>
+        <v>1954270</v>
       </c>
       <c r="F41" s="8"/>
     </row>
@@ -2904,7 +3083,7 @@
         <v>2290632</v>
       </c>
       <c r="E42" s="8">
-        <v>2094092</v>
+        <v>2029684</v>
       </c>
       <c r="F42" s="8"/>
     </row>
@@ -2922,7 +3101,7 @@
         <v>1465033.7</v>
       </c>
       <c r="E43" s="8">
-        <v>1331929</v>
+        <v>1284895</v>
       </c>
       <c r="F43" s="8"/>
     </row>
@@ -2940,7 +3119,7 @@
         <v>1331534.94</v>
       </c>
       <c r="E44" s="8">
-        <v>1264753</v>
+        <v>1190932</v>
       </c>
       <c r="F44" s="8"/>
     </row>
@@ -2958,7 +3137,7 @@
         <v>2129456</v>
       </c>
       <c r="E45" s="8">
-        <v>2058917</v>
+        <v>1891309</v>
       </c>
       <c r="F45" s="8"/>
     </row>
@@ -2976,7 +3155,7 @@
         <v>2248174</v>
       </c>
       <c r="E46" s="8">
-        <v>2103510</v>
+        <v>2020530</v>
       </c>
       <c r="F46" s="8"/>
     </row>
@@ -2994,7 +3173,7 @@
         <v>2321303</v>
       </c>
       <c r="E47" s="8">
-        <v>2221047</v>
+        <v>2149827</v>
       </c>
       <c r="F47" s="8"/>
     </row>
@@ -3012,7 +3191,7 @@
         <v>2368097</v>
       </c>
       <c r="E48" s="8">
-        <v>2247760</v>
+        <v>2180930</v>
       </c>
       <c r="F48" s="8"/>
     </row>
@@ -3030,7 +3209,7 @@
         <v>2376839</v>
       </c>
       <c r="E49" s="8">
-        <v>2270208</v>
+        <v>2208506</v>
       </c>
       <c r="F49" s="8"/>
     </row>
@@ -3048,7 +3227,7 @@
         <v>2378145</v>
       </c>
       <c r="E50" s="8">
-        <v>2319187</v>
+        <v>2247447</v>
       </c>
       <c r="F50" s="8"/>
     </row>
@@ -3066,7 +3245,7 @@
         <v>2344259.7142857141</v>
       </c>
       <c r="E51" s="8">
-        <v>2294630</v>
+        <v>2219267</v>
       </c>
       <c r="F51" s="8"/>
     </row>
@@ -3084,7 +3263,7 @@
         <v>2442710</v>
       </c>
       <c r="E52" s="8">
-        <v>2391466</v>
+        <v>2319328</v>
       </c>
       <c r="F52" s="8"/>
     </row>
@@ -3102,7 +3281,7 @@
         <v>2391289</v>
       </c>
       <c r="E53" s="11">
-        <v>2361017</v>
+        <v>2274497</v>
       </c>
       <c r="F53" s="11"/>
     </row>
@@ -3120,27 +3299,27 @@
         <v>2386839</v>
       </c>
       <c r="E54" s="11">
-        <v>2348017</v>
+        <v>2264447</v>
       </c>
       <c r="F54" s="10"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="21">
+      <c r="B55" s="19">
         <v>187</v>
       </c>
-      <c r="C55" s="21">
+      <c r="C55" s="19">
         <v>360911</v>
       </c>
-      <c r="D55" s="22">
+      <c r="D55" s="20">
         <v>2414443</v>
       </c>
-      <c r="E55" s="21">
-        <v>2386339</v>
-      </c>
-      <c r="F55" s="21"/>
+      <c r="E55" s="19">
+        <v>2304591</v>
+      </c>
+      <c r="F55" s="19"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
@@ -3156,27 +3335,27 @@
         <v>2356203</v>
       </c>
       <c r="E56" s="8">
-        <v>2326435</v>
+        <v>2251915</v>
       </c>
       <c r="F56" s="8"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="21" t="s">
+      <c r="A57" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B57" s="22">
+      <c r="B57" s="20">
         <v>180</v>
       </c>
-      <c r="C57" s="22">
+      <c r="C57" s="20">
         <v>351313</v>
       </c>
-      <c r="D57" s="22">
+      <c r="D57" s="20">
         <v>2329923</v>
       </c>
-      <c r="E57" s="22">
-        <v>2321963</v>
-      </c>
-      <c r="F57" s="21"/>
+      <c r="E57" s="20">
+        <v>2221205</v>
+      </c>
+      <c r="F57" s="19"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
@@ -3192,7 +3371,7 @@
         <v>2336559</v>
       </c>
       <c r="E58" s="8">
-        <v>2332259</v>
+        <v>2229117</v>
       </c>
       <c r="F58" s="8"/>
     </row>
@@ -3201,305 +3380,304 @@
         <v>64</v>
       </c>
       <c r="B59" s="11">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C59" s="11">
-        <v>351985</v>
-      </c>
-      <c r="D59" s="11">
-        <v>2305267</v>
-      </c>
-      <c r="E59" s="11">
-        <v>2358863</v>
-      </c>
-      <c r="F59" s="13"/>
-    </row>
-    <row r="60" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>353935</v>
+      </c>
+      <c r="D59" s="21">
+        <v>2315917</v>
+      </c>
+      <c r="E59" s="21">
+        <v>2248479</v>
+      </c>
+      <c r="F59" s="11"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="13">
+        <v>182</v>
+      </c>
+      <c r="C60" s="13">
+        <v>357961</v>
+      </c>
+      <c r="D60" s="21">
+        <v>2397963</v>
+      </c>
+      <c r="E60" s="21">
+        <v>2315015</v>
+      </c>
+      <c r="F60" s="13"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B60" s="13">
-        <v>176</v>
-      </c>
-      <c r="C60" s="13">
-        <v>352811</v>
-      </c>
-      <c r="D60" s="13">
-        <v>2368413</v>
-      </c>
-      <c r="E60" s="13">
-        <v>2370981</v>
-      </c>
-      <c r="F60" s="13"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
+      <c r="B61" s="18">
+        <v>175</v>
+      </c>
+      <c r="C61" s="13">
+        <v>352491</v>
+      </c>
+      <c r="D61" s="13">
+        <v>2369333</v>
+      </c>
+      <c r="E61" s="13">
+        <v>2300095</v>
+      </c>
+      <c r="F61" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="20"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E1" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" s="7">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C2" s="8">
-        <v>354011</v>
+        <v>354485</v>
       </c>
       <c r="D2" s="8">
-        <v>2376839</v>
+        <v>2378145</v>
       </c>
       <c r="E2" s="8">
-        <v>2270208</v>
-      </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2247447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="7">
+        <v>187</v>
+      </c>
+      <c r="C3" s="8">
+        <v>350601</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2344259.7142857141</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2219267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="7">
         <v>183</v>
       </c>
-      <c r="C3" s="8">
-        <v>354485</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2378145</v>
-      </c>
-      <c r="E3" s="8">
-        <v>2319187</v>
-      </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="7">
+      <c r="C4" s="8">
+        <v>363862</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2442710</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2319328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7">
+        <v>185</v>
+      </c>
+      <c r="C5" s="8">
+        <v>359585</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2391289</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2274497</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="7">
         <v>187</v>
       </c>
-      <c r="C4" s="8">
-        <v>350601</v>
-      </c>
-      <c r="D4" s="8">
-        <v>2344259.7142857141</v>
-      </c>
-      <c r="E4" s="8">
-        <v>2294630</v>
-      </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="7">
-        <v>183</v>
-      </c>
-      <c r="C5" s="8">
-        <v>363862</v>
-      </c>
-      <c r="D5" s="8">
-        <v>2442710</v>
-      </c>
-      <c r="E5" s="8">
-        <v>2391466</v>
-      </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="7">
-        <v>185</v>
-      </c>
       <c r="C6" s="8">
-        <v>359585</v>
+        <v>358485</v>
       </c>
       <c r="D6" s="8">
-        <v>2391289</v>
+        <v>2386839</v>
       </c>
       <c r="E6" s="8">
-        <v>2361017</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2264447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="7">
         <v>187</v>
       </c>
       <c r="C7" s="8">
-        <v>358485</v>
+        <v>360911</v>
       </c>
       <c r="D7" s="8">
-        <v>2386839</v>
+        <v>2414443</v>
       </c>
       <c r="E7" s="8">
-        <v>2348017</v>
-      </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2304591</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B8" s="7">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C8" s="8">
-        <v>360911</v>
+        <v>351649</v>
       </c>
       <c r="D8" s="8">
-        <v>2414443</v>
+        <v>2356203</v>
       </c>
       <c r="E8" s="8">
-        <v>2386339</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2251915</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B9" s="7">
+        <v>180</v>
+      </c>
+      <c r="C9" s="8">
+        <v>351313</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2329923</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2221205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="7">
         <v>182</v>
       </c>
-      <c r="C9" s="8">
-        <v>351649</v>
-      </c>
-      <c r="D9" s="8">
-        <v>2356203</v>
-      </c>
-      <c r="E9" s="8">
-        <v>2326435</v>
-      </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="7">
-        <v>180</v>
-      </c>
       <c r="C10" s="8">
-        <v>351313</v>
+        <v>353705</v>
       </c>
       <c r="D10" s="8">
-        <v>2329923</v>
+        <v>2336559</v>
       </c>
       <c r="E10" s="8">
-        <v>2321963</v>
-      </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2229117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B11" s="7">
         <v>182</v>
       </c>
       <c r="C11" s="8">
-        <v>353705</v>
+        <v>353935</v>
       </c>
       <c r="D11" s="8">
-        <v>2336559</v>
+        <v>2315917</v>
       </c>
       <c r="E11" s="8">
-        <v>2332259</v>
-      </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2248479</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" s="7">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C12" s="8">
-        <v>351985</v>
-      </c>
-      <c r="D12" s="8">
-        <v>2305267</v>
-      </c>
-      <c r="E12" s="8">
-        <v>2358863</v>
-      </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>357961</v>
+      </c>
+      <c r="D12" s="11">
+        <v>2397963</v>
+      </c>
+      <c r="E12" s="11">
+        <v>2315015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B13" s="6">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13" s="13">
-        <v>352811</v>
+        <v>352491</v>
       </c>
       <c r="D13" s="13">
-        <v>2368413</v>
+        <v>2369333</v>
       </c>
       <c r="E13" s="13">
-        <v>2370981</v>
-      </c>
-      <c r="F13" s="6"/>
+        <v>2300095</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3507,15 +3685,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -4119,18 +4297,23 @@
       <c r="B55" s="6">
         <v>15</v>
       </c>
-      <c r="C55" s="13">
+      <c r="C55" s="11">
         <v>4205</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
+      <c r="A56" s="6">
+        <v>37</v>
+      </c>
+      <c r="B56" s="6">
+        <v>16</v>
+      </c>
+      <c r="C56" s="13">
+        <v>3786</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>